<commit_message>
fixed xl rgb numbers so xl reads them all as text
</commit_message>
<xml_diff>
--- a/werners_nomenclature_of_colours.xlsx
+++ b/werners_nomenclature_of_colours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/DataSets/werner colours/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE0A07D-B62A-9D48-BBF1-F5675B7D8BB1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C70F2C0-21B4-F540-A285-66EE8EF4ADC1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1660" yWindow="940" windowWidth="26780" windowHeight="16300" xr2:uid="{481D4944-F8AF-6E4B-8027-B50ED2CF82EA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="809">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="856">
   <si>
     <t>Names</t>
   </si>
@@ -2334,9 +2334,6 @@
     <t>87662a</t>
   </si>
   <si>
-    <t>135102,42</t>
-  </si>
-  <si>
     <t>39,69,53</t>
   </si>
   <si>
@@ -2452,6 +2449,150 @@
   </si>
   <si>
     <t>Pale Brazilian Topaz</t>
+  </si>
+  <si>
+    <t>135,102,42</t>
+  </si>
+  <si>
+    <t>192,166,102</t>
+  </si>
+  <si>
+    <t>249,250,248</t>
+  </si>
+  <si>
+    <t>250,249,250</t>
+  </si>
+  <si>
+    <t>244,246,251</t>
+  </si>
+  <si>
+    <t>251,251,246</t>
+  </si>
+  <si>
+    <t>252,250,245</t>
+  </si>
+  <si>
+    <t>251,253,248</t>
+  </si>
+  <si>
+    <t>237,240,242</t>
+  </si>
+  <si>
+    <t>231,236,239</t>
+  </si>
+  <si>
+    <t>209,216,211</t>
+  </si>
+  <si>
+    <t>192,199,211</t>
+  </si>
+  <si>
+    <t>193,202,216</t>
+  </si>
+  <si>
+    <t>184,192,206</t>
+  </si>
+  <si>
+    <t>185,187,169</t>
+  </si>
+  <si>
+    <t>154,163,183</t>
+  </si>
+  <si>
+    <t>130,141,150</t>
+  </si>
+  <si>
+    <t>84,101,165</t>
+  </si>
+  <si>
+    <t>96,119,226</t>
+  </si>
+  <si>
+    <t>109,138,210</t>
+  </si>
+  <si>
+    <t>123,153,220</t>
+  </si>
+  <si>
+    <t>128,192,214</t>
+  </si>
+  <si>
+    <t>120,162,192</t>
+  </si>
+  <si>
+    <t>141,169,198</t>
+  </si>
+  <si>
+    <t>217,235,254</t>
+  </si>
+  <si>
+    <t>123,142,202</t>
+  </si>
+  <si>
+    <t>104,108,142</t>
+  </si>
+  <si>
+    <t>193,201,232</t>
+  </si>
+  <si>
+    <t>182,189,174</t>
+  </si>
+  <si>
+    <t>174,177,151</t>
+  </si>
+  <si>
+    <t>145,150,150</t>
+  </si>
+  <si>
+    <t>113,170,137</t>
+  </si>
+  <si>
+    <t>164,179,166</t>
+  </si>
+  <si>
+    <t>171,183,150</t>
+  </si>
+  <si>
+    <t>151,181,120</t>
+  </si>
+  <si>
+    <t>134,153,109</t>
+  </si>
+  <si>
+    <t>208,217,185</t>
+  </si>
+  <si>
+    <t>109,127,117</t>
+  </si>
+  <si>
+    <t>215,224,144</t>
+  </si>
+  <si>
+    <t>255,254,178</t>
+  </si>
+  <si>
+    <t>253,240,150</t>
+  </si>
+  <si>
+    <t>229,219,117</t>
+  </si>
+  <si>
+    <t>253,236,133</t>
+  </si>
+  <si>
+    <t>251,229,115</t>
+  </si>
+  <si>
+    <t>255,246,186</t>
+  </si>
+  <si>
+    <t>254,208,164</t>
+  </si>
+  <si>
+    <t>255,242,220</t>
+  </si>
+  <si>
+    <t>255,225,214</t>
   </si>
 </sst>
 </file>
@@ -2502,15 +2643,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -2838,10 +2976,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67635BE4-7229-3843-B90F-B3DF15E1318E}">
   <dimension ref="A1:N111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="F79" sqref="F79"/>
+      <selection pane="topRight" activeCell="J93" sqref="J93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2854,7 +2992,7 @@
     <col min="6" max="6" width="23.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="20.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="72.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.1640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="16.1640625" style="4" customWidth="1"/>
     <col min="10" max="10" width="19.1640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="19.83203125" style="1" customWidth="1"/>
     <col min="12" max="12" width="21.6640625" customWidth="1"/>
@@ -2887,7 +3025,7 @@
       <c r="H1" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>502</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -2900,10 +3038,10 @@
         <v>628</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -2931,11 +3069,11 @@
       <c r="H2" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>503</v>
       </c>
-      <c r="J2" s="3">
-        <v>249250248</v>
+      <c r="J2" s="4" t="s">
+        <v>810</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>504</v>
@@ -2944,10 +3082,10 @@
         <v>627</v>
       </c>
       <c r="M2" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="N2" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -2975,11 +3113,11 @@
       <c r="H3" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="J3" s="3">
-        <v>250249250</v>
+      <c r="J3" s="4" t="s">
+        <v>811</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>506</v>
@@ -2988,10 +3126,10 @@
         <v>627</v>
       </c>
       <c r="M3" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="N3" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -3019,11 +3157,11 @@
       <c r="H4" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>507</v>
       </c>
-      <c r="J4" s="3">
-        <v>244246251</v>
+      <c r="J4" s="4" t="s">
+        <v>812</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>508</v>
@@ -3032,10 +3170,10 @@
         <v>627</v>
       </c>
       <c r="M4" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="N4" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -3063,11 +3201,11 @@
       <c r="H5" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>509</v>
       </c>
-      <c r="J5" s="3">
-        <v>251251246</v>
+      <c r="J5" s="4" t="s">
+        <v>813</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>510</v>
@@ -3076,10 +3214,10 @@
         <v>627</v>
       </c>
       <c r="M5" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="N5" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -3093,7 +3231,7 @@
         <v>378</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>24</v>
@@ -3107,11 +3245,11 @@
       <c r="H6" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="4" t="s">
         <v>511</v>
       </c>
-      <c r="J6" s="3">
-        <v>252250245</v>
+      <c r="J6" s="4" t="s">
+        <v>814</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>512</v>
@@ -3120,10 +3258,10 @@
         <v>627</v>
       </c>
       <c r="M6" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="N6" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -3151,11 +3289,11 @@
       <c r="H7" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="J7" s="3">
-        <v>251253248</v>
+      <c r="J7" s="4" t="s">
+        <v>815</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>514</v>
@@ -3164,10 +3302,10 @@
         <v>627</v>
       </c>
       <c r="M7" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="N7" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -3195,11 +3333,11 @@
       <c r="H8" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="4" t="s">
         <v>515</v>
       </c>
-      <c r="J8" s="3">
-        <v>237240242</v>
+      <c r="J8" s="4" t="s">
+        <v>816</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>516</v>
@@ -3208,10 +3346,10 @@
         <v>627</v>
       </c>
       <c r="M8" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="N8" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -3239,11 +3377,11 @@
       <c r="H9" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="J9" s="3">
-        <v>231236239</v>
+      <c r="J9" s="4" t="s">
+        <v>817</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>518</v>
@@ -3252,10 +3390,10 @@
         <v>627</v>
       </c>
       <c r="M9" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="N9" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -3283,11 +3421,11 @@
       <c r="H10" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="J10" s="3">
-        <v>209216211</v>
+      <c r="J10" s="4" t="s">
+        <v>818</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>520</v>
@@ -3296,10 +3434,10 @@
         <v>627</v>
       </c>
       <c r="M10" t="s">
-        <v>789</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>792</v>
+        <v>788</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>791</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -3324,11 +3462,11 @@
       <c r="H11" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="4" t="s">
         <v>521</v>
       </c>
-      <c r="J11" s="3">
-        <v>192199211</v>
+      <c r="J11" s="4" t="s">
+        <v>819</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>522</v>
@@ -3337,10 +3475,10 @@
         <v>627</v>
       </c>
       <c r="M11" t="s">
-        <v>789</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>792</v>
+        <v>788</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>791</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -3362,11 +3500,11 @@
       <c r="H12" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="4" t="s">
         <v>523</v>
       </c>
-      <c r="J12" s="3">
-        <v>193202216</v>
+      <c r="J12" s="4" t="s">
+        <v>820</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>524</v>
@@ -3375,10 +3513,10 @@
         <v>627</v>
       </c>
       <c r="M12" t="s">
-        <v>789</v>
-      </c>
-      <c r="N12" s="6" t="s">
-        <v>792</v>
+        <v>788</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>791</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -3406,11 +3544,11 @@
       <c r="H13" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="4" t="s">
         <v>525</v>
       </c>
-      <c r="J13" s="3">
-        <v>184192206</v>
+      <c r="J13" s="4" t="s">
+        <v>821</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>526</v>
@@ -3419,10 +3557,10 @@
         <v>627</v>
       </c>
       <c r="M13" t="s">
-        <v>789</v>
-      </c>
-      <c r="N13" s="6" t="s">
-        <v>792</v>
+        <v>788</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>791</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -3450,11 +3588,11 @@
       <c r="H14" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="4" t="s">
         <v>527</v>
       </c>
-      <c r="J14" s="3">
-        <v>185187169</v>
+      <c r="J14" s="4" t="s">
+        <v>822</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>528</v>
@@ -3463,10 +3601,10 @@
         <v>627</v>
       </c>
       <c r="M14" t="s">
-        <v>789</v>
-      </c>
-      <c r="N14" s="6" t="s">
-        <v>792</v>
+        <v>788</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>791</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -3491,11 +3629,11 @@
       <c r="H15" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="4" t="s">
         <v>529</v>
       </c>
-      <c r="J15" s="3">
-        <v>154163183</v>
+      <c r="J15" s="4" t="s">
+        <v>823</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>530</v>
@@ -3504,10 +3642,10 @@
         <v>627</v>
       </c>
       <c r="M15" t="s">
-        <v>789</v>
-      </c>
-      <c r="N15" s="6" t="s">
-        <v>792</v>
+        <v>788</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>791</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -3535,11 +3673,11 @@
       <c r="H16" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="I16" s="4" t="s">
         <v>531</v>
       </c>
-      <c r="J16" s="3">
-        <v>130141150</v>
+      <c r="J16" s="4" t="s">
+        <v>824</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>532</v>
@@ -3548,10 +3686,10 @@
         <v>627</v>
       </c>
       <c r="M16" t="s">
-        <v>789</v>
-      </c>
-      <c r="N16" s="6" t="s">
-        <v>792</v>
+        <v>788</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>791</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -3579,10 +3717,10 @@
       <c r="H17" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="4" t="s">
         <v>533</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="J17" s="4" t="s">
         <v>534</v>
       </c>
       <c r="K17" s="1" t="s">
@@ -3592,10 +3730,10 @@
         <v>627</v>
       </c>
       <c r="M17" t="s">
-        <v>789</v>
-      </c>
-      <c r="N17" s="6" t="s">
-        <v>792</v>
+        <v>788</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>791</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -3620,10 +3758,10 @@
       <c r="H18" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="I18" s="5">
+      <c r="I18" s="4">
         <v>424451</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="J18" s="4" t="s">
         <v>536</v>
       </c>
       <c r="K18" s="1" t="s">
@@ -3633,10 +3771,10 @@
         <v>627</v>
       </c>
       <c r="M18" t="s">
-        <v>789</v>
-      </c>
-      <c r="N18" s="6" t="s">
-        <v>793</v>
+        <v>788</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>792</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
@@ -3664,10 +3802,10 @@
       <c r="H19" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="I19" s="4" t="s">
         <v>538</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="J19" s="4" t="s">
         <v>539</v>
       </c>
       <c r="K19" s="1" t="s">
@@ -3677,10 +3815,10 @@
         <v>627</v>
       </c>
       <c r="M19" t="s">
-        <v>789</v>
-      </c>
-      <c r="N19" s="6" t="s">
-        <v>793</v>
+        <v>788</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>792</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -3705,10 +3843,10 @@
       <c r="H20" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="I20" s="4" t="s">
         <v>541</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="J20" s="4" t="s">
         <v>542</v>
       </c>
       <c r="K20" s="1" t="s">
@@ -3718,10 +3856,10 @@
         <v>627</v>
       </c>
       <c r="M20" t="s">
-        <v>789</v>
-      </c>
-      <c r="N20" s="6" t="s">
-        <v>793</v>
+        <v>788</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>792</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -3746,10 +3884,10 @@
       <c r="H21" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="I21" s="4" t="s">
         <v>544</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="J21" s="4" t="s">
         <v>545</v>
       </c>
       <c r="K21" s="1" t="s">
@@ -3759,10 +3897,10 @@
         <v>627</v>
       </c>
       <c r="M21" t="s">
-        <v>789</v>
-      </c>
-      <c r="N21" s="6" t="s">
-        <v>793</v>
+        <v>788</v>
+      </c>
+      <c r="N21" s="5" t="s">
+        <v>792</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -3790,10 +3928,10 @@
       <c r="H22" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="I22" s="4" t="s">
         <v>547</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="J22" s="4" t="s">
         <v>548</v>
       </c>
       <c r="K22" s="1" t="s">
@@ -3803,10 +3941,10 @@
         <v>627</v>
       </c>
       <c r="M22" t="s">
-        <v>789</v>
-      </c>
-      <c r="N22" s="6" t="s">
-        <v>793</v>
+        <v>788</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>792</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
@@ -3831,10 +3969,10 @@
       <c r="H23" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="I23" s="4" t="s">
         <v>550</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="J23" s="4" t="s">
         <v>551</v>
       </c>
       <c r="K23" s="1" t="s">
@@ -3844,10 +3982,10 @@
         <v>627</v>
       </c>
       <c r="M23" t="s">
-        <v>789</v>
-      </c>
-      <c r="N23" s="6" t="s">
-        <v>793</v>
+        <v>788</v>
+      </c>
+      <c r="N23" s="5" t="s">
+        <v>792</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -3875,10 +4013,10 @@
       <c r="H24" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="I24" s="5" t="s">
+      <c r="I24" s="4" t="s">
         <v>553</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="J24" s="4" t="s">
         <v>554</v>
       </c>
       <c r="K24" s="1" t="s">
@@ -3888,10 +4026,10 @@
         <v>627</v>
       </c>
       <c r="M24" t="s">
-        <v>789</v>
-      </c>
-      <c r="N24" s="6" t="s">
-        <v>793</v>
+        <v>788</v>
+      </c>
+      <c r="N24" s="5" t="s">
+        <v>792</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -3919,10 +4057,10 @@
       <c r="H25" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="I25" s="5" t="s">
+      <c r="I25" s="4" t="s">
         <v>556</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="J25" s="4" t="s">
         <v>557</v>
       </c>
       <c r="K25" s="1" t="s">
@@ -3932,10 +4070,10 @@
         <v>627</v>
       </c>
       <c r="M25" t="s">
-        <v>789</v>
-      </c>
-      <c r="N25" s="6" t="s">
-        <v>794</v>
+        <v>788</v>
+      </c>
+      <c r="N25" s="5" t="s">
+        <v>793</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -3963,10 +4101,10 @@
       <c r="H26" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="I26" s="5">
+      <c r="I26" s="4">
         <v>60740</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="J26" s="4" t="s">
         <v>559</v>
       </c>
       <c r="K26" s="1" t="s">
@@ -3976,10 +4114,10 @@
         <v>627</v>
       </c>
       <c r="M26" t="s">
-        <v>789</v>
-      </c>
-      <c r="N26" s="6" t="s">
-        <v>794</v>
+        <v>788</v>
+      </c>
+      <c r="N26" s="5" t="s">
+        <v>793</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -4001,10 +4139,10 @@
       <c r="H27" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="I27" s="5" t="s">
+      <c r="I27" s="4" t="s">
         <v>561</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="J27" s="4" t="s">
         <v>562</v>
       </c>
       <c r="K27" s="1" t="s">
@@ -4014,10 +4152,10 @@
         <v>627</v>
       </c>
       <c r="M27" t="s">
-        <v>789</v>
-      </c>
-      <c r="N27" s="6" t="s">
-        <v>794</v>
+        <v>788</v>
+      </c>
+      <c r="N27" s="5" t="s">
+        <v>793</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -4034,7 +4172,7 @@
         <v>100</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>101</v>
@@ -4045,10 +4183,10 @@
       <c r="H28" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="I28" s="5" t="s">
+      <c r="I28" s="4" t="s">
         <v>564</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="J28" s="4" t="s">
         <v>565</v>
       </c>
       <c r="K28" s="1" t="s">
@@ -4058,10 +4196,10 @@
         <v>627</v>
       </c>
       <c r="M28" t="s">
-        <v>789</v>
-      </c>
-      <c r="N28" s="6" t="s">
-        <v>794</v>
+        <v>788</v>
+      </c>
+      <c r="N28" s="5" t="s">
+        <v>793</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -4089,11 +4227,11 @@
       <c r="H29" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="I29" s="5" t="s">
+      <c r="I29" s="4" t="s">
         <v>567</v>
       </c>
-      <c r="J29" s="3">
-        <v>84101165</v>
+      <c r="J29" s="4" t="s">
+        <v>825</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>568</v>
@@ -4102,10 +4240,10 @@
         <v>627</v>
       </c>
       <c r="M29" t="s">
-        <v>789</v>
-      </c>
-      <c r="N29" s="6" t="s">
-        <v>794</v>
+        <v>788</v>
+      </c>
+      <c r="N29" s="5" t="s">
+        <v>793</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -4133,11 +4271,11 @@
       <c r="H30" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="I30" s="5" t="s">
+      <c r="I30" s="4" t="s">
         <v>569</v>
       </c>
-      <c r="J30" s="3">
-        <v>96119226</v>
+      <c r="J30" s="4" t="s">
+        <v>826</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>570</v>
@@ -4146,10 +4284,10 @@
         <v>627</v>
       </c>
       <c r="M30" t="s">
-        <v>789</v>
-      </c>
-      <c r="N30" s="6" t="s">
-        <v>794</v>
+        <v>788</v>
+      </c>
+      <c r="N30" s="5" t="s">
+        <v>793</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -4177,11 +4315,11 @@
       <c r="H31" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="I31" s="5" t="s">
+      <c r="I31" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="J31" s="3">
-        <v>109138210</v>
+      <c r="J31" s="4" t="s">
+        <v>827</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>572</v>
@@ -4190,10 +4328,10 @@
         <v>627</v>
       </c>
       <c r="M31" t="s">
-        <v>789</v>
-      </c>
-      <c r="N31" s="6" t="s">
-        <v>794</v>
+        <v>788</v>
+      </c>
+      <c r="N31" s="5" t="s">
+        <v>793</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
@@ -4221,11 +4359,11 @@
       <c r="H32" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="I32" s="5" t="s">
+      <c r="I32" s="4" t="s">
         <v>573</v>
       </c>
-      <c r="J32" s="3">
-        <v>123153220</v>
+      <c r="J32" s="4" t="s">
+        <v>828</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>574</v>
@@ -4234,10 +4372,10 @@
         <v>627</v>
       </c>
       <c r="M32" t="s">
-        <v>789</v>
-      </c>
-      <c r="N32" s="6" t="s">
-        <v>794</v>
+        <v>788</v>
+      </c>
+      <c r="N32" s="5" t="s">
+        <v>793</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
@@ -4259,11 +4397,11 @@
       <c r="H33" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="I33" s="5" t="s">
+      <c r="I33" s="4" t="s">
         <v>575</v>
       </c>
-      <c r="J33" s="3">
-        <v>128192214</v>
+      <c r="J33" s="4" t="s">
+        <v>829</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>576</v>
@@ -4272,10 +4410,10 @@
         <v>627</v>
       </c>
       <c r="M33" t="s">
-        <v>789</v>
-      </c>
-      <c r="N33" s="6" t="s">
-        <v>794</v>
+        <v>788</v>
+      </c>
+      <c r="N33" s="5" t="s">
+        <v>793</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -4300,11 +4438,11 @@
       <c r="H34" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="I34" s="5" t="s">
+      <c r="I34" s="4" t="s">
         <v>577</v>
       </c>
-      <c r="J34" s="3">
-        <v>120162192</v>
+      <c r="J34" s="4" t="s">
+        <v>830</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>578</v>
@@ -4313,10 +4451,10 @@
         <v>627</v>
       </c>
       <c r="M34" t="s">
-        <v>789</v>
-      </c>
-      <c r="N34" s="6" t="s">
-        <v>794</v>
+        <v>788</v>
+      </c>
+      <c r="N34" s="5" t="s">
+        <v>793</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -4344,11 +4482,11 @@
       <c r="H35" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="I35" s="5" t="s">
+      <c r="I35" s="4" t="s">
         <v>579</v>
       </c>
-      <c r="J35" s="3">
-        <v>141169198</v>
+      <c r="J35" s="4" t="s">
+        <v>831</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>580</v>
@@ -4357,10 +4495,10 @@
         <v>626</v>
       </c>
       <c r="M35" t="s">
-        <v>789</v>
-      </c>
-      <c r="N35" s="6" t="s">
-        <v>794</v>
+        <v>788</v>
+      </c>
+      <c r="N35" s="5" t="s">
+        <v>793</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -4388,11 +4526,11 @@
       <c r="H36" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="I36" s="5" t="s">
+      <c r="I36" s="4" t="s">
         <v>581</v>
       </c>
-      <c r="J36" s="3">
-        <v>217235254</v>
+      <c r="J36" s="4" t="s">
+        <v>832</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>582</v>
@@ -4401,10 +4539,10 @@
         <v>626</v>
       </c>
       <c r="M36" t="s">
-        <v>789</v>
-      </c>
-      <c r="N36" s="6" t="s">
-        <v>795</v>
+        <v>788</v>
+      </c>
+      <c r="N36" s="5" t="s">
+        <v>794</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -4429,11 +4567,11 @@
       <c r="H37" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="I37" s="5" t="s">
+      <c r="I37" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="J37" s="3">
-        <v>123142202</v>
+      <c r="J37" s="4" t="s">
+        <v>833</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>584</v>
@@ -4442,10 +4580,10 @@
         <v>626</v>
       </c>
       <c r="M37" t="s">
-        <v>789</v>
-      </c>
-      <c r="N37" s="6" t="s">
-        <v>795</v>
+        <v>788</v>
+      </c>
+      <c r="N37" s="5" t="s">
+        <v>794</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -4470,7 +4608,7 @@
       <c r="H38" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="I38" s="5" t="s">
+      <c r="I38" s="4" t="s">
         <v>585</v>
       </c>
       <c r="J38" s="1" t="s">
@@ -4483,10 +4621,10 @@
         <v>626</v>
       </c>
       <c r="M38" t="s">
-        <v>789</v>
-      </c>
-      <c r="N38" s="6" t="s">
-        <v>795</v>
+        <v>788</v>
+      </c>
+      <c r="N38" s="5" t="s">
+        <v>794</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -4514,7 +4652,7 @@
       <c r="H39" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="I39" s="5" t="s">
+      <c r="I39" s="4" t="s">
         <v>588</v>
       </c>
       <c r="J39" s="1" t="s">
@@ -4527,10 +4665,10 @@
         <v>626</v>
       </c>
       <c r="M39" t="s">
-        <v>789</v>
-      </c>
-      <c r="N39" s="6" t="s">
-        <v>795</v>
+        <v>788</v>
+      </c>
+      <c r="N39" s="5" t="s">
+        <v>794</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -4555,7 +4693,7 @@
       <c r="H40" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="I40" s="5" t="s">
+      <c r="I40" s="4" t="s">
         <v>591</v>
       </c>
       <c r="J40" s="1" t="s">
@@ -4568,10 +4706,10 @@
         <v>626</v>
       </c>
       <c r="M40" t="s">
-        <v>789</v>
-      </c>
-      <c r="N40" s="6" t="s">
-        <v>795</v>
+        <v>788</v>
+      </c>
+      <c r="N40" s="5" t="s">
+        <v>794</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -4596,7 +4734,7 @@
       <c r="H41" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="I41" s="5" t="s">
+      <c r="I41" s="4" t="s">
         <v>594</v>
       </c>
       <c r="J41" s="1" t="s">
@@ -4609,10 +4747,10 @@
         <v>626</v>
       </c>
       <c r="M41" t="s">
-        <v>789</v>
-      </c>
-      <c r="N41" s="6" t="s">
-        <v>795</v>
+        <v>788</v>
+      </c>
+      <c r="N41" s="5" t="s">
+        <v>794</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -4640,7 +4778,7 @@
       <c r="H42" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="I42" s="5" t="s">
+      <c r="I42" s="4" t="s">
         <v>597</v>
       </c>
       <c r="J42" s="1" t="s">
@@ -4653,10 +4791,10 @@
         <v>626</v>
       </c>
       <c r="M42" t="s">
-        <v>789</v>
-      </c>
-      <c r="N42" s="6" t="s">
-        <v>795</v>
+        <v>788</v>
+      </c>
+      <c r="N42" s="5" t="s">
+        <v>794</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -4681,7 +4819,7 @@
       <c r="H43" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="I43" s="5" t="s">
+      <c r="I43" s="4" t="s">
         <v>600</v>
       </c>
       <c r="J43" s="1" t="s">
@@ -4694,10 +4832,10 @@
         <v>626</v>
       </c>
       <c r="M43" t="s">
-        <v>789</v>
-      </c>
-      <c r="N43" s="6" t="s">
-        <v>795</v>
+        <v>788</v>
+      </c>
+      <c r="N43" s="5" t="s">
+        <v>794</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -4725,11 +4863,11 @@
       <c r="H44" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="I44" s="5" t="s">
+      <c r="I44" s="4" t="s">
         <v>603</v>
       </c>
-      <c r="J44" s="3">
-        <v>193201232</v>
+      <c r="J44" s="4" t="s">
+        <v>835</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>604</v>
@@ -4738,10 +4876,10 @@
         <v>626</v>
       </c>
       <c r="M44" t="s">
-        <v>789</v>
-      </c>
-      <c r="N44" s="6" t="s">
-        <v>795</v>
+        <v>788</v>
+      </c>
+      <c r="N44" s="5" t="s">
+        <v>794</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -4769,11 +4907,11 @@
       <c r="H45" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="I45" s="5" t="s">
+      <c r="I45" s="4" t="s">
         <v>605</v>
       </c>
-      <c r="J45" s="3">
-        <v>104108142</v>
+      <c r="J45" s="4" t="s">
+        <v>834</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>606</v>
@@ -4782,10 +4920,10 @@
         <v>626</v>
       </c>
       <c r="M45" t="s">
-        <v>789</v>
-      </c>
-      <c r="N45" s="6" t="s">
-        <v>795</v>
+        <v>788</v>
+      </c>
+      <c r="N45" s="5" t="s">
+        <v>794</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
@@ -4807,7 +4945,7 @@
       <c r="H46" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="I46" s="5" t="s">
+      <c r="I46" s="4" t="s">
         <v>607</v>
       </c>
       <c r="J46" s="1" t="s">
@@ -4820,10 +4958,10 @@
         <v>619</v>
       </c>
       <c r="M46" t="s">
-        <v>789</v>
-      </c>
-      <c r="N46" s="6" t="s">
-        <v>795</v>
+        <v>788</v>
+      </c>
+      <c r="N46" s="5" t="s">
+        <v>794</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
@@ -4851,11 +4989,11 @@
       <c r="H47" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="I47" s="5" t="s">
+      <c r="I47" s="4" t="s">
         <v>610</v>
       </c>
-      <c r="J47" s="3">
-        <v>182189174</v>
+      <c r="J47" s="4" t="s">
+        <v>836</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>611</v>
@@ -4864,10 +5002,10 @@
         <v>619</v>
       </c>
       <c r="M47" t="s">
-        <v>789</v>
-      </c>
-      <c r="N47" s="6" t="s">
-        <v>796</v>
+        <v>788</v>
+      </c>
+      <c r="N47" s="5" t="s">
+        <v>795</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -4895,11 +5033,11 @@
       <c r="H48" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="I48" s="5" t="s">
+      <c r="I48" s="4" t="s">
         <v>612</v>
       </c>
-      <c r="J48" s="3">
-        <v>174177151</v>
+      <c r="J48" s="4" t="s">
+        <v>837</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>613</v>
@@ -4908,10 +5046,10 @@
         <v>619</v>
       </c>
       <c r="M48" t="s">
-        <v>789</v>
-      </c>
-      <c r="N48" s="6" t="s">
-        <v>796</v>
+        <v>788</v>
+      </c>
+      <c r="N48" s="5" t="s">
+        <v>795</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -4936,11 +5074,11 @@
       <c r="H49" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="I49" s="5" t="s">
+      <c r="I49" s="4" t="s">
         <v>614</v>
       </c>
-      <c r="J49" s="3">
-        <v>145150150</v>
+      <c r="J49" s="4" t="s">
+        <v>838</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>615</v>
@@ -4949,10 +5087,10 @@
         <v>619</v>
       </c>
       <c r="M49" t="s">
-        <v>789</v>
-      </c>
-      <c r="N49" s="6" t="s">
-        <v>796</v>
+        <v>788</v>
+      </c>
+      <c r="N49" s="5" t="s">
+        <v>795</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -4980,7 +5118,7 @@
       <c r="H50" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="I50" s="5" t="s">
+      <c r="I50" s="4" t="s">
         <v>616</v>
       </c>
       <c r="J50" s="1" t="s">
@@ -4993,10 +5131,10 @@
         <v>619</v>
       </c>
       <c r="M50" t="s">
-        <v>789</v>
-      </c>
-      <c r="N50" s="6" t="s">
-        <v>796</v>
+        <v>788</v>
+      </c>
+      <c r="N50" s="5" t="s">
+        <v>795</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -5021,11 +5159,11 @@
       <c r="H51" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="I51" s="5" t="s">
+      <c r="I51" s="4" t="s">
         <v>620</v>
       </c>
-      <c r="J51" s="3">
-        <v>113170137</v>
+      <c r="J51" s="4" t="s">
+        <v>839</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>621</v>
@@ -5034,10 +5172,10 @@
         <v>619</v>
       </c>
       <c r="M51" t="s">
-        <v>789</v>
-      </c>
-      <c r="N51" s="6" t="s">
-        <v>796</v>
+        <v>788</v>
+      </c>
+      <c r="N51" s="5" t="s">
+        <v>795</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -5065,11 +5203,11 @@
       <c r="H52" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="I52" s="5" t="s">
+      <c r="I52" s="4" t="s">
         <v>622</v>
       </c>
-      <c r="J52" s="3">
-        <v>164179166</v>
+      <c r="J52" s="4" t="s">
+        <v>840</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>623</v>
@@ -5078,10 +5216,10 @@
         <v>619</v>
       </c>
       <c r="M52" t="s">
-        <v>789</v>
-      </c>
-      <c r="N52" s="6" t="s">
-        <v>796</v>
+        <v>788</v>
+      </c>
+      <c r="N52" s="5" t="s">
+        <v>795</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -5106,11 +5244,11 @@
       <c r="H53" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="I53" s="5" t="s">
+      <c r="I53" s="4" t="s">
         <v>624</v>
       </c>
-      <c r="J53" s="3">
-        <v>171183150</v>
+      <c r="J53" s="4" t="s">
+        <v>841</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>625</v>
@@ -5119,10 +5257,10 @@
         <v>619</v>
       </c>
       <c r="M53" t="s">
-        <v>789</v>
-      </c>
-      <c r="N53" s="6" t="s">
-        <v>796</v>
+        <v>788</v>
+      </c>
+      <c r="N53" s="5" t="s">
+        <v>795</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -5147,11 +5285,11 @@
       <c r="H54" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="I54" s="5" t="s">
+      <c r="I54" s="4" t="s">
         <v>631</v>
       </c>
-      <c r="J54" s="3">
-        <v>151181120</v>
+      <c r="J54" s="4" t="s">
+        <v>842</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>632</v>
@@ -5160,10 +5298,10 @@
         <v>619</v>
       </c>
       <c r="M54" t="s">
-        <v>789</v>
-      </c>
-      <c r="N54" s="6" t="s">
-        <v>796</v>
+        <v>788</v>
+      </c>
+      <c r="N54" s="5" t="s">
+        <v>795</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -5191,11 +5329,11 @@
       <c r="H55" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="I55" s="5" t="s">
+      <c r="I55" s="4" t="s">
         <v>629</v>
       </c>
-      <c r="J55" s="3">
-        <v>134153109</v>
+      <c r="J55" s="4" t="s">
+        <v>843</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>630</v>
@@ -5204,10 +5342,10 @@
         <v>626</v>
       </c>
       <c r="M55" t="s">
-        <v>789</v>
-      </c>
-      <c r="N55" s="6" t="s">
-        <v>797</v>
+        <v>788</v>
+      </c>
+      <c r="N55" s="5" t="s">
+        <v>796</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -5235,7 +5373,7 @@
       <c r="H56" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="I56" s="5" t="s">
+      <c r="I56" s="4" t="s">
         <v>633</v>
       </c>
       <c r="J56" s="1" t="s">
@@ -5248,10 +5386,10 @@
         <v>626</v>
       </c>
       <c r="M56" t="s">
-        <v>789</v>
-      </c>
-      <c r="N56" s="6" t="s">
-        <v>797</v>
+        <v>788</v>
+      </c>
+      <c r="N56" s="5" t="s">
+        <v>796</v>
       </c>
     </row>
     <row r="57" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -5276,7 +5414,7 @@
       <c r="H57" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="I57" s="5" t="s">
+      <c r="I57" s="4" t="s">
         <v>636</v>
       </c>
       <c r="J57" s="1" t="s">
@@ -5289,10 +5427,10 @@
         <v>626</v>
       </c>
       <c r="M57" t="s">
-        <v>789</v>
-      </c>
-      <c r="N57" s="6" t="s">
-        <v>797</v>
+        <v>788</v>
+      </c>
+      <c r="N57" s="5" t="s">
+        <v>796</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -5320,7 +5458,7 @@
       <c r="H58" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="I58" s="5" t="s">
+      <c r="I58" s="4" t="s">
         <v>639</v>
       </c>
       <c r="J58" s="1" t="s">
@@ -5333,10 +5471,10 @@
         <v>626</v>
       </c>
       <c r="M58" t="s">
-        <v>789</v>
-      </c>
-      <c r="N58" s="6" t="s">
-        <v>797</v>
+        <v>788</v>
+      </c>
+      <c r="N58" s="5" t="s">
+        <v>796</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -5364,11 +5502,11 @@
       <c r="H59" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="I59" s="5" t="s">
+      <c r="I59" s="4" t="s">
         <v>642</v>
       </c>
-      <c r="J59" s="3">
-        <v>208217185</v>
+      <c r="J59" s="4" t="s">
+        <v>844</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>643</v>
@@ -5377,10 +5515,10 @@
         <v>626</v>
       </c>
       <c r="M59" t="s">
-        <v>789</v>
-      </c>
-      <c r="N59" s="6" t="s">
-        <v>797</v>
+        <v>788</v>
+      </c>
+      <c r="N59" s="5" t="s">
+        <v>796</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
@@ -5405,11 +5543,11 @@
       <c r="H60" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="I60" s="5" t="s">
+      <c r="I60" s="4" t="s">
         <v>644</v>
       </c>
-      <c r="J60" s="3">
-        <v>109127117</v>
+      <c r="J60" s="4" t="s">
+        <v>845</v>
       </c>
       <c r="K60" s="1" t="s">
         <v>645</v>
@@ -5418,10 +5556,10 @@
         <v>626</v>
       </c>
       <c r="M60" t="s">
-        <v>789</v>
-      </c>
-      <c r="N60" s="6" t="s">
-        <v>797</v>
+        <v>788</v>
+      </c>
+      <c r="N60" s="5" t="s">
+        <v>796</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -5449,7 +5587,7 @@
       <c r="H61" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="I61" s="5" t="s">
+      <c r="I61" s="4" t="s">
         <v>646</v>
       </c>
       <c r="J61" s="1" t="s">
@@ -5462,10 +5600,10 @@
         <v>626</v>
       </c>
       <c r="M61" t="s">
-        <v>789</v>
-      </c>
-      <c r="N61" s="6" t="s">
-        <v>797</v>
+        <v>788</v>
+      </c>
+      <c r="N61" s="5" t="s">
+        <v>796</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -5493,11 +5631,11 @@
       <c r="H62" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="I62" s="5" t="s">
+      <c r="I62" s="4" t="s">
         <v>649</v>
       </c>
-      <c r="J62" s="3">
-        <v>215224144</v>
+      <c r="J62" s="4" t="s">
+        <v>846</v>
       </c>
       <c r="K62" s="1" t="s">
         <v>650</v>
@@ -5506,10 +5644,10 @@
         <v>626</v>
       </c>
       <c r="M62" t="s">
-        <v>789</v>
-      </c>
-      <c r="N62" s="6" t="s">
-        <v>797</v>
+        <v>788</v>
+      </c>
+      <c r="N62" s="5" t="s">
+        <v>796</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -5537,7 +5675,7 @@
       <c r="H63" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="I63" s="5" t="s">
+      <c r="I63" s="4" t="s">
         <v>651</v>
       </c>
       <c r="J63" s="1" t="s">
@@ -5550,10 +5688,10 @@
         <v>626</v>
       </c>
       <c r="M63" t="s">
-        <v>789</v>
-      </c>
-      <c r="N63" s="6" t="s">
-        <v>798</v>
+        <v>788</v>
+      </c>
+      <c r="N63" s="5" t="s">
+        <v>797</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -5581,11 +5719,11 @@
       <c r="H64" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="I64" s="5" t="s">
+      <c r="I64" s="4" t="s">
         <v>654</v>
       </c>
-      <c r="J64" s="3">
-        <v>255254178</v>
+      <c r="J64" s="4" t="s">
+        <v>847</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>655</v>
@@ -5594,10 +5732,10 @@
         <v>626</v>
       </c>
       <c r="M64" t="s">
-        <v>789</v>
-      </c>
-      <c r="N64" s="6" t="s">
-        <v>798</v>
+        <v>788</v>
+      </c>
+      <c r="N64" s="5" t="s">
+        <v>797</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -5625,7 +5763,7 @@
       <c r="H65" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="I65" s="5" t="s">
+      <c r="I65" s="4" t="s">
         <v>656</v>
       </c>
       <c r="J65" s="1" t="s">
@@ -5638,10 +5776,10 @@
         <v>626</v>
       </c>
       <c r="M65" t="s">
-        <v>789</v>
-      </c>
-      <c r="N65" s="6" t="s">
-        <v>798</v>
+        <v>788</v>
+      </c>
+      <c r="N65" s="5" t="s">
+        <v>797</v>
       </c>
     </row>
     <row r="66" spans="1:14" ht="96" x14ac:dyDescent="0.2">
@@ -5658,7 +5796,7 @@
         <v>226</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>227</v>
@@ -5669,7 +5807,7 @@
       <c r="H66" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="I66" s="5" t="s">
+      <c r="I66" s="4" t="s">
         <v>659</v>
       </c>
       <c r="J66" s="1" t="s">
@@ -5682,10 +5820,10 @@
         <v>626</v>
       </c>
       <c r="M66" t="s">
-        <v>789</v>
-      </c>
-      <c r="N66" s="6" t="s">
-        <v>798</v>
+        <v>788</v>
+      </c>
+      <c r="N66" s="5" t="s">
+        <v>797</v>
       </c>
     </row>
     <row r="67" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -5713,7 +5851,7 @@
       <c r="H67" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="I67" s="5" t="s">
+      <c r="I67" s="4" t="s">
         <v>662</v>
       </c>
       <c r="J67" s="1" t="s">
@@ -5726,10 +5864,10 @@
         <v>626</v>
       </c>
       <c r="M67" t="s">
-        <v>789</v>
-      </c>
-      <c r="N67" s="6" t="s">
-        <v>798</v>
+        <v>788</v>
+      </c>
+      <c r="N67" s="5" t="s">
+        <v>797</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
@@ -5754,7 +5892,7 @@
       <c r="H68" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="I68" s="5" t="s">
+      <c r="I68" s="4" t="s">
         <v>665</v>
       </c>
       <c r="J68" s="1" t="s">
@@ -5767,10 +5905,10 @@
         <v>626</v>
       </c>
       <c r="M68" t="s">
-        <v>789</v>
-      </c>
-      <c r="N68" s="6" t="s">
-        <v>798</v>
+        <v>788</v>
+      </c>
+      <c r="N68" s="5" t="s">
+        <v>797</v>
       </c>
     </row>
     <row r="69" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -5795,7 +5933,7 @@
       <c r="H69" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="I69" s="5" t="s">
+      <c r="I69" s="4" t="s">
         <v>668</v>
       </c>
       <c r="J69" s="1" t="s">
@@ -5808,10 +5946,10 @@
         <v>626</v>
       </c>
       <c r="M69" t="s">
-        <v>789</v>
-      </c>
-      <c r="N69" s="6" t="s">
-        <v>798</v>
+        <v>788</v>
+      </c>
+      <c r="N69" s="5" t="s">
+        <v>797</v>
       </c>
     </row>
     <row r="70" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -5836,7 +5974,7 @@
       <c r="H70" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="I70" s="5" t="s">
+      <c r="I70" s="4" t="s">
         <v>671</v>
       </c>
       <c r="J70" s="1" t="s">
@@ -5849,10 +5987,10 @@
         <v>626</v>
       </c>
       <c r="M70" t="s">
-        <v>789</v>
-      </c>
-      <c r="N70" s="6" t="s">
-        <v>799</v>
+        <v>788</v>
+      </c>
+      <c r="N70" s="5" t="s">
+        <v>798</v>
       </c>
     </row>
     <row r="71" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -5877,7 +6015,7 @@
       <c r="H71" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="I71" s="5" t="s">
+      <c r="I71" s="4" t="s">
         <v>674</v>
       </c>
       <c r="J71" s="1" t="s">
@@ -5890,10 +6028,10 @@
         <v>626</v>
       </c>
       <c r="M71" t="s">
-        <v>789</v>
-      </c>
-      <c r="N71" s="6" t="s">
-        <v>799</v>
+        <v>788</v>
+      </c>
+      <c r="N71" s="5" t="s">
+        <v>798</v>
       </c>
     </row>
     <row r="72" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -5921,11 +6059,11 @@
       <c r="H72" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="I72" s="5" t="s">
+      <c r="I72" s="4" t="s">
         <v>677</v>
       </c>
-      <c r="J72" s="3">
-        <v>253240150</v>
+      <c r="J72" s="4" t="s">
+        <v>848</v>
       </c>
       <c r="K72" s="1" t="s">
         <v>678</v>
@@ -5934,10 +6072,10 @@
         <v>626</v>
       </c>
       <c r="M72" t="s">
-        <v>789</v>
-      </c>
-      <c r="N72" s="6" t="s">
-        <v>799</v>
+        <v>788</v>
+      </c>
+      <c r="N72" s="5" t="s">
+        <v>798</v>
       </c>
     </row>
     <row r="73" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -5965,11 +6103,11 @@
       <c r="H73" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="I73" s="5" t="s">
+      <c r="I73" s="4" t="s">
         <v>679</v>
       </c>
-      <c r="J73" s="3">
-        <v>229219117</v>
+      <c r="J73" s="4" t="s">
+        <v>849</v>
       </c>
       <c r="K73" s="1" t="s">
         <v>680</v>
@@ -5978,10 +6116,10 @@
         <v>626</v>
       </c>
       <c r="M73" t="s">
-        <v>789</v>
-      </c>
-      <c r="N73" s="6" t="s">
-        <v>799</v>
+        <v>788</v>
+      </c>
+      <c r="N73" s="5" t="s">
+        <v>798</v>
       </c>
     </row>
     <row r="74" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -6001,7 +6139,7 @@
         <v>253</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>216</v>
@@ -6009,11 +6147,11 @@
       <c r="H74" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="I74" s="5" t="s">
+      <c r="I74" s="4" t="s">
         <v>681</v>
       </c>
-      <c r="J74" s="3">
-        <v>253236133</v>
+      <c r="J74" s="4" t="s">
+        <v>850</v>
       </c>
       <c r="K74" s="1" t="s">
         <v>682</v>
@@ -6022,10 +6160,10 @@
         <v>626</v>
       </c>
       <c r="M74" t="s">
-        <v>789</v>
-      </c>
-      <c r="N74" s="6" t="s">
-        <v>799</v>
+        <v>788</v>
+      </c>
+      <c r="N74" s="5" t="s">
+        <v>798</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
@@ -6050,11 +6188,11 @@
       <c r="H75" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="I75" s="5" t="s">
+      <c r="I75" s="4" t="s">
         <v>683</v>
       </c>
-      <c r="J75" s="3">
-        <v>251229115</v>
+      <c r="J75" s="4" t="s">
+        <v>851</v>
       </c>
       <c r="K75" s="1" t="s">
         <v>684</v>
@@ -6063,10 +6201,10 @@
         <v>626</v>
       </c>
       <c r="M75" t="s">
-        <v>789</v>
-      </c>
-      <c r="N75" s="6" t="s">
-        <v>799</v>
+        <v>788</v>
+      </c>
+      <c r="N75" s="5" t="s">
+        <v>798</v>
       </c>
     </row>
     <row r="76" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -6091,11 +6229,11 @@
       <c r="H76" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="I76" s="5" t="s">
+      <c r="I76" s="4" t="s">
         <v>685</v>
       </c>
-      <c r="J76" s="3">
-        <v>255246186</v>
+      <c r="J76" s="4" t="s">
+        <v>852</v>
       </c>
       <c r="K76" s="1" t="s">
         <v>686</v>
@@ -6104,10 +6242,10 @@
         <v>626</v>
       </c>
       <c r="M76" t="s">
-        <v>789</v>
-      </c>
-      <c r="N76" s="6" t="s">
-        <v>799</v>
+        <v>788</v>
+      </c>
+      <c r="N76" s="5" t="s">
+        <v>798</v>
       </c>
     </row>
     <row r="77" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -6135,7 +6273,7 @@
       <c r="H77" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="I77" s="5" t="s">
+      <c r="I77" s="4" t="s">
         <v>687</v>
       </c>
       <c r="J77" s="1" t="s">
@@ -6148,10 +6286,10 @@
         <v>626</v>
       </c>
       <c r="M77" t="s">
-        <v>789</v>
-      </c>
-      <c r="N77" s="6" t="s">
-        <v>800</v>
+        <v>788</v>
+      </c>
+      <c r="N77" s="5" t="s">
+        <v>799</v>
       </c>
     </row>
     <row r="78" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -6179,7 +6317,7 @@
       <c r="H78" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="I78" s="5" t="s">
+      <c r="I78" s="4" t="s">
         <v>690</v>
       </c>
       <c r="J78" s="1" t="s">
@@ -6192,10 +6330,10 @@
         <v>626</v>
       </c>
       <c r="M78" t="s">
-        <v>789</v>
-      </c>
-      <c r="N78" s="6" t="s">
-        <v>800</v>
+        <v>788</v>
+      </c>
+      <c r="N78" s="5" t="s">
+        <v>799</v>
       </c>
     </row>
     <row r="79" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -6220,7 +6358,7 @@
       <c r="H79" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="I79" s="5" t="s">
+      <c r="I79" s="4" t="s">
         <v>693</v>
       </c>
       <c r="J79" s="1" t="s">
@@ -6233,10 +6371,10 @@
         <v>626</v>
       </c>
       <c r="M79" t="s">
-        <v>789</v>
-      </c>
-      <c r="N79" s="6" t="s">
-        <v>800</v>
+        <v>788</v>
+      </c>
+      <c r="N79" s="5" t="s">
+        <v>799</v>
       </c>
     </row>
     <row r="80" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -6256,7 +6394,7 @@
         <v>273</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>283</v>
@@ -6264,7 +6402,7 @@
       <c r="H80" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="I80" s="5" t="s">
+      <c r="I80" s="4" t="s">
         <v>696</v>
       </c>
       <c r="J80" s="1" t="s">
@@ -6277,10 +6415,10 @@
         <v>626</v>
       </c>
       <c r="M80" t="s">
-        <v>789</v>
-      </c>
-      <c r="N80" s="6" t="s">
-        <v>800</v>
+        <v>788</v>
+      </c>
+      <c r="N80" s="5" t="s">
+        <v>799</v>
       </c>
     </row>
     <row r="81" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -6305,7 +6443,7 @@
       <c r="H81" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="I81" s="5" t="s">
+      <c r="I81" s="4" t="s">
         <v>699</v>
       </c>
       <c r="J81" s="1" t="s">
@@ -6318,10 +6456,10 @@
         <v>626</v>
       </c>
       <c r="M81" t="s">
-        <v>789</v>
-      </c>
-      <c r="N81" s="6" t="s">
-        <v>800</v>
+        <v>788</v>
+      </c>
+      <c r="N81" s="5" t="s">
+        <v>799</v>
       </c>
     </row>
     <row r="82" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -6346,7 +6484,7 @@
       <c r="H82" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="I82" s="5" t="s">
+      <c r="I82" s="4" t="s">
         <v>702</v>
       </c>
       <c r="J82" s="1" t="s">
@@ -6359,10 +6497,10 @@
         <v>626</v>
       </c>
       <c r="M82" t="s">
-        <v>789</v>
-      </c>
-      <c r="N82" s="6" t="s">
-        <v>800</v>
+        <v>788</v>
+      </c>
+      <c r="N82" s="5" t="s">
+        <v>799</v>
       </c>
     </row>
     <row r="83" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -6390,7 +6528,7 @@
       <c r="H83" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="I83" s="5" t="s">
+      <c r="I83" s="4" t="s">
         <v>705</v>
       </c>
       <c r="J83" s="1" t="s">
@@ -6403,10 +6541,10 @@
         <v>627</v>
       </c>
       <c r="M83" t="s">
-        <v>789</v>
-      </c>
-      <c r="N83" s="6" t="s">
-        <v>801</v>
+        <v>788</v>
+      </c>
+      <c r="N83" s="5" t="s">
+        <v>800</v>
       </c>
     </row>
     <row r="84" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -6434,7 +6572,7 @@
       <c r="H84" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="I84" s="5" t="s">
+      <c r="I84" s="4" t="s">
         <v>708</v>
       </c>
       <c r="J84" s="1" t="s">
@@ -6447,10 +6585,10 @@
         <v>627</v>
       </c>
       <c r="M84" t="s">
-        <v>789</v>
-      </c>
-      <c r="N84" s="6" t="s">
-        <v>801</v>
+        <v>788</v>
+      </c>
+      <c r="N84" s="5" t="s">
+        <v>800</v>
       </c>
     </row>
     <row r="85" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -6478,7 +6616,7 @@
       <c r="H85" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="I85" s="5" t="s">
+      <c r="I85" s="4" t="s">
         <v>711</v>
       </c>
       <c r="J85" s="1" t="s">
@@ -6491,10 +6629,10 @@
         <v>627</v>
       </c>
       <c r="M85" t="s">
-        <v>789</v>
-      </c>
-      <c r="N85" s="6" t="s">
-        <v>801</v>
+        <v>788</v>
+      </c>
+      <c r="N85" s="5" t="s">
+        <v>800</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
@@ -6522,7 +6660,7 @@
       <c r="H86" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="I86" s="5" t="s">
+      <c r="I86" s="4" t="s">
         <v>714</v>
       </c>
       <c r="J86" s="1" t="s">
@@ -6535,10 +6673,10 @@
         <v>627</v>
       </c>
       <c r="M86" t="s">
-        <v>789</v>
-      </c>
-      <c r="N86" s="6" t="s">
-        <v>801</v>
+        <v>788</v>
+      </c>
+      <c r="N86" s="5" t="s">
+        <v>800</v>
       </c>
     </row>
     <row r="87" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -6566,7 +6704,7 @@
       <c r="H87" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="I87" s="5" t="s">
+      <c r="I87" s="4" t="s">
         <v>717</v>
       </c>
       <c r="J87" s="1" t="s">
@@ -6579,10 +6717,10 @@
         <v>627</v>
       </c>
       <c r="M87" t="s">
-        <v>789</v>
-      </c>
-      <c r="N87" s="6" t="s">
-        <v>801</v>
+        <v>788</v>
+      </c>
+      <c r="N87" s="5" t="s">
+        <v>800</v>
       </c>
     </row>
     <row r="88" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -6607,7 +6745,7 @@
       <c r="H88" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="I88" s="5" t="s">
+      <c r="I88" s="4" t="s">
         <v>720</v>
       </c>
       <c r="J88" s="1" t="s">
@@ -6620,10 +6758,10 @@
         <v>627</v>
       </c>
       <c r="M88" t="s">
-        <v>789</v>
-      </c>
-      <c r="N88" s="6" t="s">
-        <v>801</v>
+        <v>788</v>
+      </c>
+      <c r="N88" s="5" t="s">
+        <v>800</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
@@ -6651,11 +6789,11 @@
       <c r="H89" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="I89" s="5" t="s">
+      <c r="I89" s="4" t="s">
         <v>723</v>
       </c>
-      <c r="J89" s="3">
-        <v>254208164</v>
+      <c r="J89" s="4" t="s">
+        <v>853</v>
       </c>
       <c r="K89" s="1" t="s">
         <v>724</v>
@@ -6664,10 +6802,10 @@
         <v>627</v>
       </c>
       <c r="M89" t="s">
-        <v>789</v>
-      </c>
-      <c r="N89" s="6" t="s">
-        <v>801</v>
+        <v>788</v>
+      </c>
+      <c r="N89" s="5" t="s">
+        <v>800</v>
       </c>
     </row>
     <row r="90" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -6692,11 +6830,11 @@
       <c r="H90" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="I90" s="5" t="s">
+      <c r="I90" s="4" t="s">
         <v>725</v>
       </c>
-      <c r="J90" s="3">
-        <v>255242220</v>
+      <c r="J90" s="4" t="s">
+        <v>854</v>
       </c>
       <c r="K90" s="1" t="s">
         <v>726</v>
@@ -6705,10 +6843,10 @@
         <v>627</v>
       </c>
       <c r="M90" t="s">
-        <v>789</v>
-      </c>
-      <c r="N90" s="6" t="s">
-        <v>801</v>
+        <v>788</v>
+      </c>
+      <c r="N90" s="5" t="s">
+        <v>800</v>
       </c>
     </row>
     <row r="91" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -6733,11 +6871,11 @@
       <c r="H91" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="I91" s="5" t="s">
+      <c r="I91" s="4" t="s">
         <v>727</v>
       </c>
-      <c r="J91" s="3">
-        <v>255225214</v>
+      <c r="J91" s="4" t="s">
+        <v>855</v>
       </c>
       <c r="K91" s="1" t="s">
         <v>728</v>
@@ -6746,10 +6884,10 @@
         <v>627</v>
       </c>
       <c r="M91" t="s">
-        <v>789</v>
-      </c>
-      <c r="N91" s="6" t="s">
-        <v>801</v>
+        <v>788</v>
+      </c>
+      <c r="N91" s="5" t="s">
+        <v>800</v>
       </c>
     </row>
     <row r="92" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -6774,7 +6912,7 @@
       <c r="H92" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="I92" s="5" t="s">
+      <c r="I92" s="4" t="s">
         <v>729</v>
       </c>
       <c r="J92" s="1" t="s">
@@ -6787,10 +6925,10 @@
         <v>626</v>
       </c>
       <c r="M92" t="s">
-        <v>789</v>
-      </c>
-      <c r="N92" s="6" t="s">
-        <v>802</v>
+        <v>788</v>
+      </c>
+      <c r="N92" s="5" t="s">
+        <v>801</v>
       </c>
     </row>
     <row r="93" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -6815,7 +6953,7 @@
       <c r="H93" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="I93" s="5" t="s">
+      <c r="I93" s="4" t="s">
         <v>732</v>
       </c>
       <c r="J93" s="1" t="s">
@@ -6828,10 +6966,10 @@
         <v>626</v>
       </c>
       <c r="M93" t="s">
-        <v>789</v>
-      </c>
-      <c r="N93" s="6" t="s">
-        <v>802</v>
+        <v>788</v>
+      </c>
+      <c r="N93" s="5" t="s">
+        <v>801</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.2">
@@ -6853,7 +6991,7 @@
       <c r="H94" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="I94" s="5" t="s">
+      <c r="I94" s="4" t="s">
         <v>735</v>
       </c>
       <c r="J94" s="1" t="s">
@@ -6866,10 +7004,10 @@
         <v>626</v>
       </c>
       <c r="M94" t="s">
-        <v>789</v>
-      </c>
-      <c r="N94" s="6" t="s">
-        <v>802</v>
+        <v>788</v>
+      </c>
+      <c r="N94" s="5" t="s">
+        <v>801</v>
       </c>
     </row>
     <row r="95" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -6897,7 +7035,7 @@
       <c r="H95" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="I95" s="5" t="s">
+      <c r="I95" s="4" t="s">
         <v>738</v>
       </c>
       <c r="J95" s="1" t="s">
@@ -6910,10 +7048,10 @@
         <v>626</v>
       </c>
       <c r="M95" t="s">
-        <v>789</v>
-      </c>
-      <c r="N95" s="6" t="s">
-        <v>802</v>
+        <v>788</v>
+      </c>
+      <c r="N95" s="5" t="s">
+        <v>801</v>
       </c>
     </row>
     <row r="96" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -6938,7 +7076,7 @@
       <c r="H96" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="I96" s="5" t="s">
+      <c r="I96" s="4" t="s">
         <v>741</v>
       </c>
       <c r="J96" s="1" t="s">
@@ -6951,10 +7089,10 @@
         <v>626</v>
       </c>
       <c r="M96" t="s">
-        <v>789</v>
-      </c>
-      <c r="N96" s="6" t="s">
-        <v>802</v>
+        <v>788</v>
+      </c>
+      <c r="N96" s="5" t="s">
+        <v>801</v>
       </c>
     </row>
     <row r="97" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -6982,7 +7120,7 @@
       <c r="H97" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="I97" s="5" t="s">
+      <c r="I97" s="4" t="s">
         <v>744</v>
       </c>
       <c r="J97" s="1" t="s">
@@ -6995,10 +7133,10 @@
         <v>626</v>
       </c>
       <c r="M97" t="s">
-        <v>789</v>
-      </c>
-      <c r="N97" s="6" t="s">
-        <v>802</v>
+        <v>788</v>
+      </c>
+      <c r="N97" s="5" t="s">
+        <v>801</v>
       </c>
     </row>
     <row r="98" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -7023,7 +7161,7 @@
       <c r="H98" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="I98" s="5" t="s">
+      <c r="I98" s="4" t="s">
         <v>747</v>
       </c>
       <c r="J98" s="1" t="s">
@@ -7036,10 +7174,10 @@
         <v>626</v>
       </c>
       <c r="M98" t="s">
-        <v>789</v>
-      </c>
-      <c r="N98" s="6" t="s">
-        <v>802</v>
+        <v>788</v>
+      </c>
+      <c r="N98" s="5" t="s">
+        <v>801</v>
       </c>
     </row>
     <row r="99" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -7064,7 +7202,7 @@
       <c r="H99" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="I99" s="5" t="s">
+      <c r="I99" s="4" t="s">
         <v>750</v>
       </c>
       <c r="J99" s="1" t="s">
@@ -7077,10 +7215,10 @@
         <v>626</v>
       </c>
       <c r="M99" t="s">
-        <v>789</v>
-      </c>
-      <c r="N99" s="6" t="s">
-        <v>802</v>
+        <v>788</v>
+      </c>
+      <c r="N99" s="5" t="s">
+        <v>801</v>
       </c>
     </row>
     <row r="100" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -7105,7 +7243,7 @@
       <c r="H100" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="I100" s="5" t="s">
+      <c r="I100" s="4" t="s">
         <v>753</v>
       </c>
       <c r="J100" s="1" t="s">
@@ -7118,10 +7256,10 @@
         <v>626</v>
       </c>
       <c r="M100" t="s">
-        <v>789</v>
-      </c>
-      <c r="N100" s="6" t="s">
-        <v>802</v>
+        <v>788</v>
+      </c>
+      <c r="N100" s="5" t="s">
+        <v>801</v>
       </c>
     </row>
     <row r="101" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -7146,7 +7284,7 @@
       <c r="H101" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="I101" s="5" t="s">
+      <c r="I101" s="4" t="s">
         <v>756</v>
       </c>
       <c r="J101" s="1" t="s">
@@ -7159,10 +7297,10 @@
         <v>627</v>
       </c>
       <c r="M101" t="s">
-        <v>789</v>
-      </c>
-      <c r="N101" s="6" t="s">
-        <v>803</v>
+        <v>788</v>
+      </c>
+      <c r="N101" s="5" t="s">
+        <v>802</v>
       </c>
     </row>
     <row r="102" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -7190,7 +7328,7 @@
       <c r="H102" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="I102" s="5" t="s">
+      <c r="I102" s="4" t="s">
         <v>759</v>
       </c>
       <c r="J102" s="1" t="s">
@@ -7203,10 +7341,10 @@
         <v>627</v>
       </c>
       <c r="M102" t="s">
-        <v>789</v>
-      </c>
-      <c r="N102" s="7" t="s">
-        <v>803</v>
+        <v>788</v>
+      </c>
+      <c r="N102" s="6" t="s">
+        <v>802</v>
       </c>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
@@ -7231,7 +7369,7 @@
       <c r="H103" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="I103" s="5" t="s">
+      <c r="I103" s="4" t="s">
         <v>762</v>
       </c>
       <c r="J103" s="1" t="s">
@@ -7244,10 +7382,10 @@
         <v>627</v>
       </c>
       <c r="M103" t="s">
-        <v>789</v>
-      </c>
-      <c r="N103" s="7" t="s">
-        <v>803</v>
+        <v>788</v>
+      </c>
+      <c r="N103" s="6" t="s">
+        <v>802</v>
       </c>
     </row>
     <row r="104" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -7275,7 +7413,7 @@
       <c r="H104" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="I104" s="5" t="s">
+      <c r="I104" s="4" t="s">
         <v>765</v>
       </c>
       <c r="J104" s="1" t="s">
@@ -7288,10 +7426,10 @@
         <v>627</v>
       </c>
       <c r="M104" t="s">
-        <v>789</v>
-      </c>
-      <c r="N104" s="7" t="s">
-        <v>803</v>
+        <v>788</v>
+      </c>
+      <c r="N104" s="6" t="s">
+        <v>802</v>
       </c>
     </row>
     <row r="105" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -7316,23 +7454,23 @@
       <c r="H105" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="I105" s="5" t="s">
+      <c r="I105" s="4" t="s">
         <v>768</v>
       </c>
-      <c r="J105" s="3" t="s">
+      <c r="J105" s="4" t="s">
+        <v>808</v>
+      </c>
+      <c r="K105" s="1" t="s">
         <v>769</v>
-      </c>
-      <c r="K105" s="1" t="s">
-        <v>770</v>
       </c>
       <c r="L105" s="1" t="s">
         <v>627</v>
       </c>
       <c r="M105" t="s">
-        <v>789</v>
-      </c>
-      <c r="N105" s="7" t="s">
-        <v>803</v>
+        <v>788</v>
+      </c>
+      <c r="N105" s="6" t="s">
+        <v>802</v>
       </c>
     </row>
     <row r="106" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -7360,23 +7498,23 @@
       <c r="H106" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="I106" s="5" t="s">
+      <c r="I106" s="4" t="s">
+        <v>770</v>
+      </c>
+      <c r="J106" s="4" t="s">
+        <v>809</v>
+      </c>
+      <c r="K106" s="1" t="s">
         <v>771</v>
-      </c>
-      <c r="J106" s="3">
-        <v>192166102</v>
-      </c>
-      <c r="K106" s="1" t="s">
-        <v>772</v>
       </c>
       <c r="L106" s="1" t="s">
         <v>627</v>
       </c>
       <c r="M106" t="s">
-        <v>789</v>
-      </c>
-      <c r="N106" s="7" t="s">
-        <v>803</v>
+        <v>788</v>
+      </c>
+      <c r="N106" s="6" t="s">
+        <v>802</v>
       </c>
     </row>
     <row r="107" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -7401,23 +7539,23 @@
       <c r="H107" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="I107" s="5" t="s">
+      <c r="I107" s="4" t="s">
+        <v>772</v>
+      </c>
+      <c r="J107" s="1" t="s">
         <v>773</v>
       </c>
-      <c r="J107" s="1" t="s">
+      <c r="K107" s="1" t="s">
         <v>774</v>
-      </c>
-      <c r="K107" s="1" t="s">
-        <v>775</v>
       </c>
       <c r="L107" s="1" t="s">
         <v>627</v>
       </c>
       <c r="M107" t="s">
-        <v>789</v>
-      </c>
-      <c r="N107" s="7" t="s">
-        <v>803</v>
+        <v>788</v>
+      </c>
+      <c r="N107" s="6" t="s">
+        <v>802</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
@@ -7442,23 +7580,23 @@
       <c r="H108" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="I108" s="5" t="s">
+      <c r="I108" s="4" t="s">
+        <v>775</v>
+      </c>
+      <c r="J108" s="1" t="s">
         <v>776</v>
       </c>
-      <c r="J108" s="1" t="s">
+      <c r="K108" s="1" t="s">
         <v>777</v>
-      </c>
-      <c r="K108" s="1" t="s">
-        <v>778</v>
       </c>
       <c r="L108" s="1" t="s">
         <v>627</v>
       </c>
       <c r="M108" t="s">
-        <v>789</v>
-      </c>
-      <c r="N108" s="7" t="s">
-        <v>803</v>
+        <v>788</v>
+      </c>
+      <c r="N108" s="6" t="s">
+        <v>802</v>
       </c>
     </row>
     <row r="109" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -7483,23 +7621,23 @@
       <c r="H109" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="I109" s="5" t="s">
+      <c r="I109" s="4" t="s">
+        <v>778</v>
+      </c>
+      <c r="J109" s="1" t="s">
         <v>779</v>
       </c>
-      <c r="J109" s="1" t="s">
+      <c r="K109" s="1" t="s">
         <v>780</v>
-      </c>
-      <c r="K109" s="1" t="s">
-        <v>781</v>
       </c>
       <c r="L109" s="1" t="s">
         <v>627</v>
       </c>
       <c r="M109" t="s">
-        <v>789</v>
-      </c>
-      <c r="N109" s="7" t="s">
-        <v>803</v>
+        <v>788</v>
+      </c>
+      <c r="N109" s="6" t="s">
+        <v>802</v>
       </c>
     </row>
     <row r="110" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -7527,23 +7665,23 @@
       <c r="H110" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="I110" s="5" t="s">
+      <c r="I110" s="4" t="s">
+        <v>781</v>
+      </c>
+      <c r="J110" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="J110" s="1" t="s">
+      <c r="K110" s="1" t="s">
         <v>783</v>
-      </c>
-      <c r="K110" s="1" t="s">
-        <v>784</v>
       </c>
       <c r="L110" s="1" t="s">
         <v>627</v>
       </c>
       <c r="M110" t="s">
-        <v>789</v>
-      </c>
-      <c r="N110" s="7" t="s">
-        <v>803</v>
+        <v>788</v>
+      </c>
+      <c r="N110" s="6" t="s">
+        <v>802</v>
       </c>
     </row>
     <row r="111" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -7568,23 +7706,23 @@
       <c r="H111" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="I111" s="5" t="s">
+      <c r="I111" s="4" t="s">
+        <v>784</v>
+      </c>
+      <c r="J111" s="1" t="s">
         <v>785</v>
       </c>
-      <c r="J111" s="1" t="s">
+      <c r="K111" s="1" t="s">
         <v>786</v>
-      </c>
-      <c r="K111" s="1" t="s">
-        <v>787</v>
       </c>
       <c r="L111" s="1" t="s">
         <v>627</v>
       </c>
       <c r="M111" t="s">
-        <v>789</v>
-      </c>
-      <c r="N111" s="7" t="s">
-        <v>803</v>
+        <v>788</v>
+      </c>
+      <c r="N111" s="6" t="s">
+        <v>802</v>
       </c>
     </row>
   </sheetData>
@@ -7617,5 +7755,6 @@
     <hyperlink ref="N101" r:id="rId26" xr:uid="{587D31B9-4F61-064F-B3E1-BFA5BA05ABC3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added straight uncorrected rgbs
</commit_message>
<xml_diff>
--- a/werners_nomenclature_of_colours.xlsx
+++ b/werners_nomenclature_of_colours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/DataSets/werner colours/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FD25B4-4F72-8547-A43E-59DB8C42BD07}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780A51CE-475C-B047-8CB3-F1703DB63CF1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1660" yWindow="940" windowWidth="26780" windowHeight="16300" xr2:uid="{481D4944-F8AF-6E4B-8027-B50ED2CF82EA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="968">
   <si>
     <t>Names</t>
   </si>
@@ -2596,6 +2596,339 @@
   </si>
   <si>
     <t>060740</t>
+  </si>
+  <si>
+    <t>237,234,206</t>
+  </si>
+  <si>
+    <t>238,232,210</t>
+  </si>
+  <si>
+    <t>238,228,210</t>
+  </si>
+  <si>
+    <t>240,236,204</t>
+  </si>
+  <si>
+    <t>240,232,204</t>
+  </si>
+  <si>
+    <t>244,236,204</t>
+  </si>
+  <si>
+    <t>230,226,204</t>
+  </si>
+  <si>
+    <t>227,220,202</t>
+  </si>
+  <si>
+    <t>204,200,184</t>
+  </si>
+  <si>
+    <t>190,188,174</t>
+  </si>
+  <si>
+    <t>190,190,180</t>
+  </si>
+  <si>
+    <t>184,180,172</t>
+  </si>
+  <si>
+    <t>182,178,148</t>
+  </si>
+  <si>
+    <t>158,158,156</t>
+  </si>
+  <si>
+    <t>143,140,132</t>
+  </si>
+  <si>
+    <t>94,92,98</t>
+  </si>
+  <si>
+    <t>88,84,84</t>
+  </si>
+  <si>
+    <t>70,68,74</t>
+  </si>
+  <si>
+    <t>70,72,73</t>
+  </si>
+  <si>
+    <t>70,62,60</t>
+  </si>
+  <si>
+    <t>70,60,58</t>
+  </si>
+  <si>
+    <t>43,38,44</t>
+  </si>
+  <si>
+    <t>40,40,40</t>
+  </si>
+  <si>
+    <t>46,40,66</t>
+  </si>
+  <si>
+    <t>34,32,73</t>
+  </si>
+  <si>
+    <t>91,102,140</t>
+  </si>
+  <si>
+    <t>58,57,101</t>
+  </si>
+  <si>
+    <t>100,112,145</t>
+  </si>
+  <si>
+    <t>111,123,186</t>
+  </si>
+  <si>
+    <t>120,139,173</t>
+  </si>
+  <si>
+    <t>130,150,178</t>
+  </si>
+  <si>
+    <t>138,180,172</t>
+  </si>
+  <si>
+    <t>130,156,166</t>
+  </si>
+  <si>
+    <t>146,160,166</t>
+  </si>
+  <si>
+    <t>210,212,214</t>
+  </si>
+  <si>
+    <t>136,144,172</t>
+  </si>
+  <si>
+    <t>60,52,84</t>
+  </si>
+  <si>
+    <t>62,58,76</t>
+  </si>
+  <si>
+    <t>111,112,148</t>
+  </si>
+  <si>
+    <t>88,76,116</t>
+  </si>
+  <si>
+    <t>78,58,85</t>
+  </si>
+  <si>
+    <t>69,58,86</t>
+  </si>
+  <si>
+    <t>189,186,192</t>
+  </si>
+  <si>
+    <t>118,118,129</t>
+  </si>
+  <si>
+    <t>76,74,94</t>
+  </si>
+  <si>
+    <t>189,190,178</t>
+  </si>
+  <si>
+    <t>182,180,154</t>
+  </si>
+  <si>
+    <t>156,156,132</t>
+  </si>
+  <si>
+    <t>100,100,100</t>
+  </si>
+  <si>
+    <t>124,173,137</t>
+  </si>
+  <si>
+    <t>171,180,166</t>
+  </si>
+  <si>
+    <t>178,188,156</t>
+  </si>
+  <si>
+    <t>160,184,124</t>
+  </si>
+  <si>
+    <t>134,140,90</t>
+  </si>
+  <si>
+    <t>61,70,39</t>
+  </si>
+  <si>
+    <t>128,136,65</t>
+  </si>
+  <si>
+    <t>146,152,81</t>
+  </si>
+  <si>
+    <t>194,194,147</t>
+  </si>
+  <si>
+    <t>110,120,98</t>
+  </si>
+  <si>
+    <t>165,146,80</t>
+  </si>
+  <si>
+    <t>203,200,116</t>
+  </si>
+  <si>
+    <t>202,196,92</t>
+  </si>
+  <si>
+    <t>232,220,156</t>
+  </si>
+  <si>
+    <t>166,148,78</t>
+  </si>
+  <si>
+    <t>215,196,108</t>
+  </si>
+  <si>
+    <t>226,208,98</t>
+  </si>
+  <si>
+    <t>231,212,108</t>
+  </si>
+  <si>
+    <t>194,158,56</t>
+  </si>
+  <si>
+    <t>150,104,50</t>
+  </si>
+  <si>
+    <t>158,128,66</t>
+  </si>
+  <si>
+    <t>235,212,152</t>
+  </si>
+  <si>
+    <t>214,196,138</t>
+  </si>
+  <si>
+    <t>235,212,142</t>
+  </si>
+  <si>
+    <t>231,204,136</t>
+  </si>
+  <si>
+    <t>238,220,170</t>
+  </si>
+  <si>
+    <t>212,168,72</t>
+  </si>
+  <si>
+    <t>227,188,118</t>
+  </si>
+  <si>
+    <t>190,126,74</t>
+  </si>
+  <si>
+    <t>133,74,54</t>
+  </si>
+  <si>
+    <t>175,116,80</t>
+  </si>
+  <si>
+    <t>168,99,65</t>
+  </si>
+  <si>
+    <t>182,108,78</t>
+  </si>
+  <si>
+    <t>151,90,60</t>
+  </si>
+  <si>
+    <t>160,67,59</t>
+  </si>
+  <si>
+    <t>163,76,66</t>
+  </si>
+  <si>
+    <t>186,110,92</t>
+  </si>
+  <si>
+    <t>102,28,34</t>
+  </si>
+  <si>
+    <t>224,196,156</t>
+  </si>
+  <si>
+    <t>239,220,196</t>
+  </si>
+  <si>
+    <t>230,204,194</t>
+  </si>
+  <si>
+    <t>182,86,110</t>
+  </si>
+  <si>
+    <t>163,76,112</t>
+  </si>
+  <si>
+    <t>172,116,124</t>
+  </si>
+  <si>
+    <t>90,46,71</t>
+  </si>
+  <si>
+    <t>114,78,78</t>
+  </si>
+  <si>
+    <t>64,56,55</t>
+  </si>
+  <si>
+    <t>136,116,112</t>
+  </si>
+  <si>
+    <t>76,60,61</t>
+  </si>
+  <si>
+    <t>101,62,54</t>
+  </si>
+  <si>
+    <t>122,78,58</t>
+  </si>
+  <si>
+    <t>95,60,60</t>
+  </si>
+  <si>
+    <t>88,68,60</t>
+  </si>
+  <si>
+    <t>114,78,64</t>
+  </si>
+  <si>
+    <t>138,110,72</t>
+  </si>
+  <si>
+    <t>186,158,112</t>
+  </si>
+  <si>
+    <t>83,68,58</t>
+  </si>
+  <si>
+    <t>134,118,92</t>
+  </si>
+  <si>
+    <t>150,132,110</t>
+  </si>
+  <si>
+    <t>119,100,84</t>
+  </si>
+  <si>
+    <t>70,65,56</t>
+  </si>
+  <si>
+    <t>colour value - rgb</t>
   </si>
 </sst>
 </file>
@@ -2646,7 +2979,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2662,6 +2995,7 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2977,12 +3311,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67635BE4-7229-3843-B90F-B3DF15E1318E}">
-  <dimension ref="A1:N111"/>
+  <dimension ref="A1:O111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="I26" sqref="I26"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2995,15 +3329,16 @@
     <col min="6" max="6" width="23.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="20.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="72.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.1640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="19.1640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="19.83203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="21.6640625" customWidth="1"/>
-    <col min="13" max="13" width="60" customWidth="1"/>
-    <col min="14" max="14" width="76.83203125" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="19.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.83203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="21.6640625" customWidth="1"/>
+    <col min="14" max="14" width="60" customWidth="1"/>
+    <col min="15" max="15" width="76.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -3028,26 +3363,29 @@
       <c r="H1" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="7" t="s">
+        <v>967</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>502</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>628</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>787</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>803</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3072,26 +3410,29 @@
       <c r="H2" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" t="s">
+        <v>857</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>503</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>810</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>627</v>
       </c>
-      <c r="M2" t="s">
-        <v>788</v>
-      </c>
       <c r="N2" t="s">
+        <v>788</v>
+      </c>
+      <c r="O2" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3116,26 +3457,29 @@
       <c r="H3" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" t="s">
+        <v>858</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>811</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>627</v>
       </c>
-      <c r="M3" t="s">
-        <v>788</v>
-      </c>
       <c r="N3" t="s">
+        <v>788</v>
+      </c>
+      <c r="O3" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3160,26 +3504,29 @@
       <c r="H4" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" t="s">
+        <v>859</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>507</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>812</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>627</v>
       </c>
-      <c r="M4" t="s">
-        <v>788</v>
-      </c>
       <c r="N4" t="s">
+        <v>788</v>
+      </c>
+      <c r="O4" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3204,26 +3551,29 @@
       <c r="H5" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" t="s">
+        <v>860</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>509</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>813</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>627</v>
       </c>
-      <c r="M5" t="s">
-        <v>788</v>
-      </c>
       <c r="N5" t="s">
+        <v>788</v>
+      </c>
+      <c r="O5" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3248,26 +3598,29 @@
       <c r="H6" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" t="s">
+        <v>861</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>511</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>814</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>627</v>
       </c>
-      <c r="M6" t="s">
-        <v>788</v>
-      </c>
       <c r="N6" t="s">
+        <v>788</v>
+      </c>
+      <c r="O6" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3292,26 +3645,29 @@
       <c r="H7" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" t="s">
+        <v>862</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="K7" s="4" t="s">
         <v>815</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>627</v>
       </c>
-      <c r="M7" t="s">
-        <v>788</v>
-      </c>
       <c r="N7" t="s">
+        <v>788</v>
+      </c>
+      <c r="O7" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3336,26 +3692,29 @@
       <c r="H8" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" t="s">
+        <v>863</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>515</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="K8" s="4" t="s">
         <v>816</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>627</v>
       </c>
-      <c r="M8" t="s">
-        <v>788</v>
-      </c>
       <c r="N8" t="s">
+        <v>788</v>
+      </c>
+      <c r="O8" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3380,26 +3739,29 @@
       <c r="H9" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" t="s">
+        <v>864</v>
+      </c>
+      <c r="J9" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="K9" s="4" t="s">
         <v>817</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>518</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>627</v>
       </c>
-      <c r="M9" t="s">
-        <v>788</v>
-      </c>
       <c r="N9" t="s">
+        <v>788</v>
+      </c>
+      <c r="O9" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3424,26 +3786,29 @@
       <c r="H10" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" t="s">
+        <v>865</v>
+      </c>
+      <c r="J10" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="K10" s="4" t="s">
         <v>818</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>627</v>
       </c>
-      <c r="M10" t="s">
-        <v>788</v>
-      </c>
-      <c r="N10" s="5" t="s">
+      <c r="N10" t="s">
+        <v>788</v>
+      </c>
+      <c r="O10" s="5" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3465,26 +3830,29 @@
       <c r="H11" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" t="s">
+        <v>866</v>
+      </c>
+      <c r="J11" s="4" t="s">
         <v>521</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="K11" s="4" t="s">
         <v>819</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>627</v>
       </c>
-      <c r="M11" t="s">
-        <v>788</v>
-      </c>
-      <c r="N11" s="5" t="s">
+      <c r="N11" t="s">
+        <v>788</v>
+      </c>
+      <c r="O11" s="5" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3503,26 +3871,29 @@
       <c r="H12" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" t="s">
+        <v>867</v>
+      </c>
+      <c r="J12" s="4" t="s">
         <v>523</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="K12" s="4" t="s">
         <v>820</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>627</v>
       </c>
-      <c r="M12" t="s">
-        <v>788</v>
-      </c>
-      <c r="N12" s="5" t="s">
+      <c r="N12" t="s">
+        <v>788</v>
+      </c>
+      <c r="O12" s="5" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3547,26 +3918,29 @@
       <c r="H13" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" t="s">
+        <v>868</v>
+      </c>
+      <c r="J13" s="4" t="s">
         <v>525</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="K13" s="4" t="s">
         <v>821</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>627</v>
       </c>
-      <c r="M13" t="s">
-        <v>788</v>
-      </c>
-      <c r="N13" s="5" t="s">
+      <c r="N13" t="s">
+        <v>788</v>
+      </c>
+      <c r="O13" s="5" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3591,26 +3965,29 @@
       <c r="H14" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" t="s">
+        <v>869</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>527</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="K14" s="4" t="s">
         <v>822</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>627</v>
       </c>
-      <c r="M14" t="s">
-        <v>788</v>
-      </c>
-      <c r="N14" s="5" t="s">
+      <c r="N14" t="s">
+        <v>788</v>
+      </c>
+      <c r="O14" s="5" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3632,26 +4009,29 @@
       <c r="H15" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" t="s">
+        <v>870</v>
+      </c>
+      <c r="J15" s="4" t="s">
         <v>529</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="K15" s="4" t="s">
         <v>823</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>627</v>
       </c>
-      <c r="M15" t="s">
-        <v>788</v>
-      </c>
-      <c r="N15" s="5" t="s">
+      <c r="N15" t="s">
+        <v>788</v>
+      </c>
+      <c r="O15" s="5" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3676,26 +4056,29 @@
       <c r="H16" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" t="s">
+        <v>871</v>
+      </c>
+      <c r="J16" s="4" t="s">
         <v>531</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="K16" s="4" t="s">
         <v>824</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>627</v>
       </c>
-      <c r="M16" t="s">
-        <v>788</v>
-      </c>
-      <c r="N16" s="5" t="s">
+      <c r="N16" t="s">
+        <v>788</v>
+      </c>
+      <c r="O16" s="5" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -3720,26 +4103,29 @@
       <c r="H17" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" t="s">
+        <v>872</v>
+      </c>
+      <c r="J17" s="4" t="s">
         <v>533</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="K17" s="4" t="s">
         <v>534</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>627</v>
       </c>
-      <c r="M17" t="s">
-        <v>788</v>
-      </c>
-      <c r="N17" s="5" t="s">
+      <c r="N17" t="s">
+        <v>788</v>
+      </c>
+      <c r="O17" s="5" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -3761,26 +4147,29 @@
       <c r="H18" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I18" t="s">
+        <v>873</v>
+      </c>
+      <c r="J18" s="4">
         <v>424451</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="K18" s="4" t="s">
         <v>536</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>627</v>
       </c>
-      <c r="M18" t="s">
-        <v>788</v>
-      </c>
-      <c r="N18" s="5" t="s">
+      <c r="N18" t="s">
+        <v>788</v>
+      </c>
+      <c r="O18" s="5" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -3805,26 +4194,29 @@
       <c r="H19" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" t="s">
+        <v>874</v>
+      </c>
+      <c r="J19" s="4" t="s">
         <v>538</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="K19" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>540</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>627</v>
       </c>
-      <c r="M19" t="s">
-        <v>788</v>
-      </c>
-      <c r="N19" s="5" t="s">
+      <c r="N19" t="s">
+        <v>788</v>
+      </c>
+      <c r="O19" s="5" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -3846,26 +4238,29 @@
       <c r="H20" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="I20" t="s">
+        <v>875</v>
+      </c>
+      <c r="J20" s="4" t="s">
         <v>541</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="K20" s="4" t="s">
         <v>542</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>627</v>
       </c>
-      <c r="M20" t="s">
-        <v>788</v>
-      </c>
-      <c r="N20" s="5" t="s">
+      <c r="N20" t="s">
+        <v>788</v>
+      </c>
+      <c r="O20" s="5" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -3887,26 +4282,29 @@
       <c r="H21" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="I21" s="4" t="s">
+      <c r="I21" t="s">
+        <v>876</v>
+      </c>
+      <c r="J21" s="4" t="s">
         <v>544</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="K21" s="4" t="s">
         <v>545</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>627</v>
       </c>
-      <c r="M21" t="s">
-        <v>788</v>
-      </c>
-      <c r="N21" s="5" t="s">
+      <c r="N21" t="s">
+        <v>788</v>
+      </c>
+      <c r="O21" s="5" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3931,26 +4329,29 @@
       <c r="H22" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="I22" t="s">
+        <v>877</v>
+      </c>
+      <c r="J22" s="4" t="s">
         <v>547</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="K22" s="4" t="s">
         <v>548</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="L22" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>627</v>
       </c>
-      <c r="M22" t="s">
-        <v>788</v>
-      </c>
-      <c r="N22" s="5" t="s">
+      <c r="N22" t="s">
+        <v>788</v>
+      </c>
+      <c r="O22" s="5" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -3972,26 +4373,29 @@
       <c r="H23" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="I23" t="s">
+        <v>878</v>
+      </c>
+      <c r="J23" s="4" t="s">
         <v>550</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="K23" s="4" t="s">
         <v>551</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="L23" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>627</v>
       </c>
-      <c r="M23" t="s">
-        <v>788</v>
-      </c>
-      <c r="N23" s="5" t="s">
+      <c r="N23" t="s">
+        <v>788</v>
+      </c>
+      <c r="O23" s="5" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -4016,26 +4420,29 @@
       <c r="H24" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="I24" s="4" t="s">
+      <c r="I24" t="s">
+        <v>879</v>
+      </c>
+      <c r="J24" s="4" t="s">
         <v>553</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="K24" s="4" t="s">
         <v>554</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="L24" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>627</v>
       </c>
-      <c r="M24" t="s">
-        <v>788</v>
-      </c>
-      <c r="N24" s="5" t="s">
+      <c r="N24" t="s">
+        <v>788</v>
+      </c>
+      <c r="O24" s="5" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -4060,26 +4467,29 @@
       <c r="H25" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="I25" s="4" t="s">
+      <c r="I25" t="s">
+        <v>880</v>
+      </c>
+      <c r="J25" s="4" t="s">
         <v>556</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="K25" s="4" t="s">
         <v>557</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>627</v>
       </c>
-      <c r="M25" t="s">
-        <v>788</v>
-      </c>
-      <c r="N25" s="5" t="s">
+      <c r="N25" t="s">
+        <v>788</v>
+      </c>
+      <c r="O25" s="5" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -4104,26 +4514,29 @@
       <c r="H26" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="I26" s="4" t="s">
+      <c r="I26" t="s">
+        <v>881</v>
+      </c>
+      <c r="J26" s="4" t="s">
         <v>856</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="K26" s="4" t="s">
         <v>559</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="L26" s="1" t="s">
         <v>560</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>627</v>
       </c>
-      <c r="M26" t="s">
-        <v>788</v>
-      </c>
-      <c r="N26" s="5" t="s">
+      <c r="N26" t="s">
+        <v>788</v>
+      </c>
+      <c r="O26" s="5" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -4142,26 +4555,29 @@
       <c r="H27" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="I27" t="s">
+        <v>882</v>
+      </c>
+      <c r="J27" s="4" t="s">
         <v>561</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="K27" s="4" t="s">
         <v>562</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="L27" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>627</v>
       </c>
-      <c r="M27" t="s">
-        <v>788</v>
-      </c>
-      <c r="N27" s="5" t="s">
+      <c r="N27" t="s">
+        <v>788</v>
+      </c>
+      <c r="O27" s="5" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -4186,26 +4602,29 @@
       <c r="H28" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="I28" s="4" t="s">
+      <c r="I28" t="s">
+        <v>883</v>
+      </c>
+      <c r="J28" s="4" t="s">
         <v>564</v>
       </c>
-      <c r="J28" s="4" t="s">
+      <c r="K28" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="L28" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>627</v>
       </c>
-      <c r="M28" t="s">
-        <v>788</v>
-      </c>
-      <c r="N28" s="5" t="s">
+      <c r="N28" t="s">
+        <v>788</v>
+      </c>
+      <c r="O28" s="5" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -4230,26 +4649,29 @@
       <c r="H29" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="I29" s="4" t="s">
+      <c r="I29" t="s">
+        <v>884</v>
+      </c>
+      <c r="J29" s="4" t="s">
         <v>567</v>
       </c>
-      <c r="J29" s="4" t="s">
+      <c r="K29" s="4" t="s">
         <v>825</v>
       </c>
-      <c r="K29" s="1" t="s">
+      <c r="L29" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>627</v>
       </c>
-      <c r="M29" t="s">
-        <v>788</v>
-      </c>
-      <c r="N29" s="5" t="s">
+      <c r="N29" t="s">
+        <v>788</v>
+      </c>
+      <c r="O29" s="5" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -4274,26 +4696,29 @@
       <c r="H30" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="I30" s="4" t="s">
+      <c r="I30" t="s">
+        <v>885</v>
+      </c>
+      <c r="J30" s="4" t="s">
         <v>569</v>
       </c>
-      <c r="J30" s="4" t="s">
+      <c r="K30" s="4" t="s">
         <v>826</v>
       </c>
-      <c r="K30" s="1" t="s">
+      <c r="L30" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>627</v>
       </c>
-      <c r="M30" t="s">
-        <v>788</v>
-      </c>
-      <c r="N30" s="5" t="s">
+      <c r="N30" t="s">
+        <v>788</v>
+      </c>
+      <c r="O30" s="5" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -4318,26 +4743,29 @@
       <c r="H31" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="I31" s="4" t="s">
+      <c r="I31" t="s">
+        <v>886</v>
+      </c>
+      <c r="J31" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="K31" s="4" t="s">
         <v>827</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="L31" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="L31" t="s">
+      <c r="M31" t="s">
         <v>627</v>
       </c>
-      <c r="M31" t="s">
-        <v>788</v>
-      </c>
-      <c r="N31" s="5" t="s">
+      <c r="N31" t="s">
+        <v>788</v>
+      </c>
+      <c r="O31" s="5" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -4362,26 +4790,29 @@
       <c r="H32" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="I32" t="s">
+        <v>887</v>
+      </c>
+      <c r="J32" s="4" t="s">
         <v>573</v>
       </c>
-      <c r="J32" s="4" t="s">
+      <c r="K32" s="4" t="s">
         <v>828</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="L32" s="1" t="s">
         <v>574</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M32" t="s">
         <v>627</v>
       </c>
-      <c r="M32" t="s">
-        <v>788</v>
-      </c>
-      <c r="N32" s="5" t="s">
+      <c r="N32" t="s">
+        <v>788</v>
+      </c>
+      <c r="O32" s="5" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -4400,26 +4831,29 @@
       <c r="H33" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="I33" s="4" t="s">
+      <c r="I33" t="s">
+        <v>888</v>
+      </c>
+      <c r="J33" s="4" t="s">
         <v>575</v>
       </c>
-      <c r="J33" s="4" t="s">
+      <c r="K33" s="4" t="s">
         <v>829</v>
       </c>
-      <c r="K33" s="1" t="s">
+      <c r="L33" s="1" t="s">
         <v>576</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>627</v>
       </c>
-      <c r="M33" t="s">
-        <v>788</v>
-      </c>
-      <c r="N33" s="5" t="s">
+      <c r="N33" t="s">
+        <v>788</v>
+      </c>
+      <c r="O33" s="5" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -4441,26 +4875,29 @@
       <c r="H34" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="I34" s="4" t="s">
+      <c r="I34" t="s">
+        <v>889</v>
+      </c>
+      <c r="J34" s="4" t="s">
         <v>577</v>
       </c>
-      <c r="J34" s="4" t="s">
+      <c r="K34" s="4" t="s">
         <v>830</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="L34" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
         <v>627</v>
       </c>
-      <c r="M34" t="s">
-        <v>788</v>
-      </c>
-      <c r="N34" s="5" t="s">
+      <c r="N34" t="s">
+        <v>788</v>
+      </c>
+      <c r="O34" s="5" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -4485,26 +4922,29 @@
       <c r="H35" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="I35" s="4" t="s">
+      <c r="I35" t="s">
+        <v>890</v>
+      </c>
+      <c r="J35" s="4" t="s">
         <v>579</v>
       </c>
-      <c r="J35" s="4" t="s">
+      <c r="K35" s="4" t="s">
         <v>831</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="L35" s="1" t="s">
         <v>580</v>
       </c>
-      <c r="L35" t="s">
+      <c r="M35" t="s">
         <v>626</v>
       </c>
-      <c r="M35" t="s">
-        <v>788</v>
-      </c>
-      <c r="N35" s="5" t="s">
+      <c r="N35" t="s">
+        <v>788</v>
+      </c>
+      <c r="O35" s="5" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -4529,26 +4969,29 @@
       <c r="H36" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="I36" s="4" t="s">
+      <c r="I36" t="s">
+        <v>891</v>
+      </c>
+      <c r="J36" s="4" t="s">
         <v>581</v>
       </c>
-      <c r="J36" s="4" t="s">
+      <c r="K36" s="4" t="s">
         <v>832</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="L36" s="1" t="s">
         <v>582</v>
       </c>
-      <c r="L36" t="s">
+      <c r="M36" t="s">
         <v>626</v>
       </c>
-      <c r="M36" t="s">
-        <v>788</v>
-      </c>
-      <c r="N36" s="5" t="s">
+      <c r="N36" t="s">
+        <v>788</v>
+      </c>
+      <c r="O36" s="5" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -4570,26 +5013,29 @@
       <c r="H37" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="I37" s="4" t="s">
+      <c r="I37" t="s">
+        <v>892</v>
+      </c>
+      <c r="J37" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="J37" s="4" t="s">
+      <c r="K37" s="4" t="s">
         <v>833</v>
       </c>
-      <c r="K37" s="1" t="s">
+      <c r="L37" s="1" t="s">
         <v>584</v>
       </c>
-      <c r="L37" t="s">
+      <c r="M37" t="s">
         <v>626</v>
       </c>
-      <c r="M37" t="s">
-        <v>788</v>
-      </c>
-      <c r="N37" s="5" t="s">
+      <c r="N37" t="s">
+        <v>788</v>
+      </c>
+      <c r="O37" s="5" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -4611,26 +5057,29 @@
       <c r="H38" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="I38" s="4" t="s">
+      <c r="I38" t="s">
+        <v>893</v>
+      </c>
+      <c r="J38" s="4" t="s">
         <v>585</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="K38" s="1" t="s">
         <v>586</v>
       </c>
-      <c r="K38" s="1" t="s">
+      <c r="L38" s="1" t="s">
         <v>587</v>
       </c>
-      <c r="L38" t="s">
+      <c r="M38" t="s">
         <v>626</v>
       </c>
-      <c r="M38" t="s">
-        <v>788</v>
-      </c>
-      <c r="N38" s="5" t="s">
+      <c r="N38" t="s">
+        <v>788</v>
+      </c>
+      <c r="O38" s="5" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -4655,26 +5104,29 @@
       <c r="H39" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="I39" s="4" t="s">
+      <c r="I39" t="s">
+        <v>894</v>
+      </c>
+      <c r="J39" s="4" t="s">
         <v>588</v>
       </c>
-      <c r="J39" s="1" t="s">
+      <c r="K39" s="1" t="s">
         <v>589</v>
       </c>
-      <c r="K39" s="1" t="s">
+      <c r="L39" s="1" t="s">
         <v>590</v>
       </c>
-      <c r="L39" t="s">
+      <c r="M39" t="s">
         <v>626</v>
       </c>
-      <c r="M39" t="s">
-        <v>788</v>
-      </c>
-      <c r="N39" s="5" t="s">
+      <c r="N39" t="s">
+        <v>788</v>
+      </c>
+      <c r="O39" s="5" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -4696,26 +5148,29 @@
       <c r="H40" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="I40" s="4" t="s">
+      <c r="I40" t="s">
+        <v>895</v>
+      </c>
+      <c r="J40" s="4" t="s">
         <v>591</v>
       </c>
-      <c r="J40" s="1" t="s">
+      <c r="K40" s="1" t="s">
         <v>592</v>
       </c>
-      <c r="K40" s="1" t="s">
+      <c r="L40" s="1" t="s">
         <v>593</v>
       </c>
-      <c r="L40" t="s">
+      <c r="M40" t="s">
         <v>626</v>
       </c>
-      <c r="M40" t="s">
-        <v>788</v>
-      </c>
-      <c r="N40" s="5" t="s">
+      <c r="N40" t="s">
+        <v>788</v>
+      </c>
+      <c r="O40" s="5" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -4737,26 +5192,29 @@
       <c r="H41" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="I41" s="4" t="s">
+      <c r="I41" t="s">
+        <v>896</v>
+      </c>
+      <c r="J41" s="4" t="s">
         <v>594</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="K41" s="1" t="s">
         <v>595</v>
       </c>
-      <c r="K41" s="1" t="s">
+      <c r="L41" s="1" t="s">
         <v>596</v>
       </c>
-      <c r="L41" t="s">
+      <c r="M41" t="s">
         <v>626</v>
       </c>
-      <c r="M41" t="s">
-        <v>788</v>
-      </c>
-      <c r="N41" s="5" t="s">
+      <c r="N41" t="s">
+        <v>788</v>
+      </c>
+      <c r="O41" s="5" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -4781,26 +5239,29 @@
       <c r="H42" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="I42" s="4" t="s">
+      <c r="I42" t="s">
+        <v>897</v>
+      </c>
+      <c r="J42" s="4" t="s">
         <v>597</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="K42" s="1" t="s">
         <v>598</v>
       </c>
-      <c r="K42" s="1" t="s">
+      <c r="L42" s="1" t="s">
         <v>599</v>
       </c>
-      <c r="L42" t="s">
+      <c r="M42" t="s">
         <v>626</v>
       </c>
-      <c r="M42" t="s">
-        <v>788</v>
-      </c>
-      <c r="N42" s="5" t="s">
+      <c r="N42" t="s">
+        <v>788</v>
+      </c>
+      <c r="O42" s="5" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -4822,26 +5283,29 @@
       <c r="H43" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="I43" s="4" t="s">
+      <c r="I43" t="s">
+        <v>898</v>
+      </c>
+      <c r="J43" s="4" t="s">
         <v>600</v>
       </c>
-      <c r="J43" s="1" t="s">
+      <c r="K43" s="1" t="s">
         <v>601</v>
       </c>
-      <c r="K43" s="1" t="s">
+      <c r="L43" s="1" t="s">
         <v>602</v>
       </c>
-      <c r="L43" t="s">
+      <c r="M43" t="s">
         <v>626</v>
       </c>
-      <c r="M43" t="s">
-        <v>788</v>
-      </c>
-      <c r="N43" s="5" t="s">
+      <c r="N43" t="s">
+        <v>788</v>
+      </c>
+      <c r="O43" s="5" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -4866,26 +5330,29 @@
       <c r="H44" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="I44" s="4" t="s">
+      <c r="I44" t="s">
+        <v>899</v>
+      </c>
+      <c r="J44" s="4" t="s">
         <v>603</v>
       </c>
-      <c r="J44" s="4" t="s">
+      <c r="K44" s="4" t="s">
         <v>835</v>
       </c>
-      <c r="K44" s="1" t="s">
+      <c r="L44" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="L44" t="s">
+      <c r="M44" t="s">
         <v>626</v>
       </c>
-      <c r="M44" t="s">
-        <v>788</v>
-      </c>
-      <c r="N44" s="5" t="s">
+      <c r="N44" t="s">
+        <v>788</v>
+      </c>
+      <c r="O44" s="5" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -4910,26 +5377,29 @@
       <c r="H45" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="I45" s="4" t="s">
+      <c r="I45" t="s">
+        <v>900</v>
+      </c>
+      <c r="J45" s="4" t="s">
         <v>605</v>
       </c>
-      <c r="J45" s="4" t="s">
+      <c r="K45" s="4" t="s">
         <v>834</v>
       </c>
-      <c r="K45" s="1" t="s">
+      <c r="L45" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="L45" t="s">
+      <c r="M45" t="s">
         <v>626</v>
       </c>
-      <c r="M45" t="s">
-        <v>788</v>
-      </c>
-      <c r="N45" s="5" t="s">
+      <c r="N45" t="s">
+        <v>788</v>
+      </c>
+      <c r="O45" s="5" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -4948,26 +5418,29 @@
       <c r="H46" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="I46" s="4" t="s">
+      <c r="I46" t="s">
+        <v>901</v>
+      </c>
+      <c r="J46" s="4" t="s">
         <v>607</v>
       </c>
-      <c r="J46" s="1" t="s">
+      <c r="K46" s="1" t="s">
         <v>608</v>
       </c>
-      <c r="K46" s="1" t="s">
+      <c r="L46" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="L46" s="1" t="s">
+      <c r="M46" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="M46" t="s">
-        <v>788</v>
-      </c>
-      <c r="N46" s="5" t="s">
+      <c r="N46" t="s">
+        <v>788</v>
+      </c>
+      <c r="O46" s="5" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -4992,26 +5465,29 @@
       <c r="H47" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="I47" s="4" t="s">
+      <c r="I47" t="s">
+        <v>902</v>
+      </c>
+      <c r="J47" s="4" t="s">
         <v>610</v>
       </c>
-      <c r="J47" s="4" t="s">
+      <c r="K47" s="4" t="s">
         <v>836</v>
       </c>
-      <c r="K47" s="1" t="s">
+      <c r="L47" s="1" t="s">
         <v>611</v>
       </c>
-      <c r="L47" s="1" t="s">
+      <c r="M47" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="M47" t="s">
-        <v>788</v>
-      </c>
-      <c r="N47" s="5" t="s">
+      <c r="N47" t="s">
+        <v>788</v>
+      </c>
+      <c r="O47" s="5" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -5036,26 +5512,29 @@
       <c r="H48" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="I48" s="4" t="s">
+      <c r="I48" t="s">
+        <v>903</v>
+      </c>
+      <c r="J48" s="4" t="s">
         <v>612</v>
       </c>
-      <c r="J48" s="4" t="s">
+      <c r="K48" s="4" t="s">
         <v>837</v>
       </c>
-      <c r="K48" s="1" t="s">
+      <c r="L48" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="L48" s="1" t="s">
+      <c r="M48" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="M48" t="s">
-        <v>788</v>
-      </c>
-      <c r="N48" s="5" t="s">
+      <c r="N48" t="s">
+        <v>788</v>
+      </c>
+      <c r="O48" s="5" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -5077,26 +5556,29 @@
       <c r="H49" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="I49" s="4" t="s">
+      <c r="I49" t="s">
+        <v>904</v>
+      </c>
+      <c r="J49" s="4" t="s">
         <v>614</v>
       </c>
-      <c r="J49" s="4" t="s">
+      <c r="K49" s="4" t="s">
         <v>838</v>
       </c>
-      <c r="K49" s="1" t="s">
+      <c r="L49" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="L49" s="1" t="s">
+      <c r="M49" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="M49" t="s">
-        <v>788</v>
-      </c>
-      <c r="N49" s="5" t="s">
+      <c r="N49" t="s">
+        <v>788</v>
+      </c>
+      <c r="O49" s="5" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -5121,26 +5603,29 @@
       <c r="H50" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="I50" s="4" t="s">
+      <c r="I50" t="s">
+        <v>905</v>
+      </c>
+      <c r="J50" s="4" t="s">
         <v>616</v>
       </c>
-      <c r="J50" s="1" t="s">
+      <c r="K50" s="1" t="s">
         <v>617</v>
       </c>
-      <c r="K50" s="1" t="s">
+      <c r="L50" s="1" t="s">
         <v>618</v>
       </c>
-      <c r="L50" s="1" t="s">
+      <c r="M50" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="M50" t="s">
-        <v>788</v>
-      </c>
-      <c r="N50" s="5" t="s">
+      <c r="N50" t="s">
+        <v>788</v>
+      </c>
+      <c r="O50" s="5" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -5162,26 +5647,29 @@
       <c r="H51" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="I51" s="4" t="s">
+      <c r="I51" t="s">
+        <v>906</v>
+      </c>
+      <c r="J51" s="4" t="s">
         <v>620</v>
       </c>
-      <c r="J51" s="4" t="s">
+      <c r="K51" s="4" t="s">
         <v>839</v>
       </c>
-      <c r="K51" s="1" t="s">
+      <c r="L51" s="1" t="s">
         <v>621</v>
       </c>
-      <c r="L51" s="1" t="s">
+      <c r="M51" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="M51" t="s">
-        <v>788</v>
-      </c>
-      <c r="N51" s="5" t="s">
+      <c r="N51" t="s">
+        <v>788</v>
+      </c>
+      <c r="O51" s="5" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -5206,26 +5694,29 @@
       <c r="H52" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="I52" s="4" t="s">
+      <c r="I52" t="s">
+        <v>907</v>
+      </c>
+      <c r="J52" s="4" t="s">
         <v>622</v>
       </c>
-      <c r="J52" s="4" t="s">
+      <c r="K52" s="4" t="s">
         <v>840</v>
       </c>
-      <c r="K52" s="1" t="s">
+      <c r="L52" s="1" t="s">
         <v>623</v>
       </c>
-      <c r="L52" s="1" t="s">
+      <c r="M52" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="M52" t="s">
-        <v>788</v>
-      </c>
-      <c r="N52" s="5" t="s">
+      <c r="N52" t="s">
+        <v>788</v>
+      </c>
+      <c r="O52" s="5" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -5247,26 +5738,29 @@
       <c r="H53" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="I53" s="4" t="s">
+      <c r="I53" t="s">
+        <v>908</v>
+      </c>
+      <c r="J53" s="4" t="s">
         <v>624</v>
       </c>
-      <c r="J53" s="4" t="s">
+      <c r="K53" s="4" t="s">
         <v>841</v>
       </c>
-      <c r="K53" s="1" t="s">
+      <c r="L53" s="1" t="s">
         <v>625</v>
       </c>
-      <c r="L53" s="1" t="s">
+      <c r="M53" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="M53" t="s">
-        <v>788</v>
-      </c>
-      <c r="N53" s="5" t="s">
+      <c r="N53" t="s">
+        <v>788</v>
+      </c>
+      <c r="O53" s="5" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -5288,26 +5782,29 @@
       <c r="H54" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="I54" s="4" t="s">
+      <c r="I54" t="s">
+        <v>909</v>
+      </c>
+      <c r="J54" s="4" t="s">
         <v>631</v>
       </c>
-      <c r="J54" s="4" t="s">
+      <c r="K54" s="4" t="s">
         <v>842</v>
       </c>
-      <c r="K54" s="1" t="s">
+      <c r="L54" s="1" t="s">
         <v>632</v>
       </c>
-      <c r="L54" s="1" t="s">
+      <c r="M54" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="M54" t="s">
-        <v>788</v>
-      </c>
-      <c r="N54" s="5" t="s">
+      <c r="N54" t="s">
+        <v>788</v>
+      </c>
+      <c r="O54" s="5" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -5332,26 +5829,29 @@
       <c r="H55" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="I55" s="4" t="s">
+      <c r="I55" t="s">
+        <v>910</v>
+      </c>
+      <c r="J55" s="4" t="s">
         <v>629</v>
       </c>
-      <c r="J55" s="4" t="s">
+      <c r="K55" s="4" t="s">
         <v>843</v>
       </c>
-      <c r="K55" s="1" t="s">
+      <c r="L55" s="1" t="s">
         <v>630</v>
       </c>
-      <c r="L55" s="1" t="s">
+      <c r="M55" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M55" t="s">
-        <v>788</v>
-      </c>
-      <c r="N55" s="5" t="s">
+      <c r="N55" t="s">
+        <v>788</v>
+      </c>
+      <c r="O55" s="5" t="s">
         <v>796</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -5376,26 +5876,29 @@
       <c r="H56" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="I56" s="4" t="s">
+      <c r="I56" t="s">
+        <v>911</v>
+      </c>
+      <c r="J56" s="4" t="s">
         <v>633</v>
       </c>
-      <c r="J56" s="1" t="s">
+      <c r="K56" s="1" t="s">
         <v>634</v>
       </c>
-      <c r="K56" s="1" t="s">
+      <c r="L56" s="1" t="s">
         <v>635</v>
       </c>
-      <c r="L56" s="1" t="s">
+      <c r="M56" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M56" t="s">
-        <v>788</v>
-      </c>
-      <c r="N56" s="5" t="s">
+      <c r="N56" t="s">
+        <v>788</v>
+      </c>
+      <c r="O56" s="5" t="s">
         <v>796</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -5417,26 +5920,29 @@
       <c r="H57" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="I57" s="4" t="s">
+      <c r="I57" t="s">
+        <v>912</v>
+      </c>
+      <c r="J57" s="4" t="s">
         <v>636</v>
       </c>
-      <c r="J57" s="1" t="s">
+      <c r="K57" s="1" t="s">
         <v>637</v>
       </c>
-      <c r="K57" s="1" t="s">
+      <c r="L57" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="L57" s="1" t="s">
+      <c r="M57" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M57" t="s">
-        <v>788</v>
-      </c>
-      <c r="N57" s="5" t="s">
+      <c r="N57" t="s">
+        <v>788</v>
+      </c>
+      <c r="O57" s="5" t="s">
         <v>796</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -5461,26 +5967,29 @@
       <c r="H58" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="I58" s="4" t="s">
+      <c r="I58" t="s">
+        <v>913</v>
+      </c>
+      <c r="J58" s="4" t="s">
         <v>639</v>
       </c>
-      <c r="J58" s="1" t="s">
+      <c r="K58" s="1" t="s">
         <v>640</v>
       </c>
-      <c r="K58" s="1" t="s">
+      <c r="L58" s="1" t="s">
         <v>641</v>
       </c>
-      <c r="L58" s="1" t="s">
+      <c r="M58" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M58" t="s">
-        <v>788</v>
-      </c>
-      <c r="N58" s="5" t="s">
+      <c r="N58" t="s">
+        <v>788</v>
+      </c>
+      <c r="O58" s="5" t="s">
         <v>796</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -5505,26 +6014,29 @@
       <c r="H59" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="I59" s="4" t="s">
+      <c r="I59" t="s">
+        <v>914</v>
+      </c>
+      <c r="J59" s="4" t="s">
         <v>642</v>
       </c>
-      <c r="J59" s="4" t="s">
+      <c r="K59" s="4" t="s">
         <v>844</v>
       </c>
-      <c r="K59" s="1" t="s">
+      <c r="L59" s="1" t="s">
         <v>643</v>
       </c>
-      <c r="L59" s="1" t="s">
+      <c r="M59" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M59" t="s">
-        <v>788</v>
-      </c>
-      <c r="N59" s="5" t="s">
+      <c r="N59" t="s">
+        <v>788</v>
+      </c>
+      <c r="O59" s="5" t="s">
         <v>796</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -5546,26 +6058,29 @@
       <c r="H60" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="I60" s="4" t="s">
+      <c r="I60" t="s">
+        <v>915</v>
+      </c>
+      <c r="J60" s="4" t="s">
         <v>644</v>
       </c>
-      <c r="J60" s="4" t="s">
+      <c r="K60" s="4" t="s">
         <v>845</v>
       </c>
-      <c r="K60" s="1" t="s">
+      <c r="L60" s="1" t="s">
         <v>645</v>
       </c>
-      <c r="L60" s="1" t="s">
+      <c r="M60" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M60" t="s">
-        <v>788</v>
-      </c>
-      <c r="N60" s="5" t="s">
+      <c r="N60" t="s">
+        <v>788</v>
+      </c>
+      <c r="O60" s="5" t="s">
         <v>796</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -5590,26 +6105,29 @@
       <c r="H61" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="I61" s="4" t="s">
+      <c r="I61" t="s">
+        <v>916</v>
+      </c>
+      <c r="J61" s="4" t="s">
         <v>646</v>
       </c>
-      <c r="J61" s="1" t="s">
+      <c r="K61" s="1" t="s">
         <v>647</v>
       </c>
-      <c r="K61" s="1" t="s">
+      <c r="L61" s="1" t="s">
         <v>648</v>
       </c>
-      <c r="L61" s="1" t="s">
+      <c r="M61" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M61" t="s">
-        <v>788</v>
-      </c>
-      <c r="N61" s="5" t="s">
+      <c r="N61" t="s">
+        <v>788</v>
+      </c>
+      <c r="O61" s="5" t="s">
         <v>796</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -5634,26 +6152,29 @@
       <c r="H62" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="I62" s="4" t="s">
+      <c r="I62" t="s">
+        <v>917</v>
+      </c>
+      <c r="J62" s="4" t="s">
         <v>649</v>
       </c>
-      <c r="J62" s="4" t="s">
+      <c r="K62" s="4" t="s">
         <v>846</v>
       </c>
-      <c r="K62" s="1" t="s">
+      <c r="L62" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="L62" s="1" t="s">
+      <c r="M62" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M62" t="s">
-        <v>788</v>
-      </c>
-      <c r="N62" s="5" t="s">
+      <c r="N62" t="s">
+        <v>788</v>
+      </c>
+      <c r="O62" s="5" t="s">
         <v>796</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -5678,26 +6199,29 @@
       <c r="H63" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="I63" s="4" t="s">
+      <c r="I63" t="s">
+        <v>918</v>
+      </c>
+      <c r="J63" s="4" t="s">
         <v>651</v>
       </c>
-      <c r="J63" s="1" t="s">
+      <c r="K63" s="1" t="s">
         <v>652</v>
       </c>
-      <c r="K63" s="1" t="s">
+      <c r="L63" s="1" t="s">
         <v>653</v>
       </c>
-      <c r="L63" s="1" t="s">
+      <c r="M63" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M63" t="s">
-        <v>788</v>
-      </c>
-      <c r="N63" s="5" t="s">
+      <c r="N63" t="s">
+        <v>788</v>
+      </c>
+      <c r="O63" s="5" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -5722,26 +6246,29 @@
       <c r="H64" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="I64" s="4" t="s">
+      <c r="I64" t="s">
+        <v>919</v>
+      </c>
+      <c r="J64" s="4" t="s">
         <v>654</v>
       </c>
-      <c r="J64" s="4" t="s">
+      <c r="K64" s="4" t="s">
         <v>847</v>
       </c>
-      <c r="K64" s="1" t="s">
+      <c r="L64" s="1" t="s">
         <v>655</v>
       </c>
-      <c r="L64" s="1" t="s">
+      <c r="M64" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M64" t="s">
-        <v>788</v>
-      </c>
-      <c r="N64" s="5" t="s">
+      <c r="N64" t="s">
+        <v>788</v>
+      </c>
+      <c r="O64" s="5" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -5766,26 +6293,29 @@
       <c r="H65" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="I65" s="4" t="s">
+      <c r="I65" t="s">
+        <v>920</v>
+      </c>
+      <c r="J65" s="4" t="s">
         <v>656</v>
       </c>
-      <c r="J65" s="1" t="s">
+      <c r="K65" s="1" t="s">
         <v>657</v>
       </c>
-      <c r="K65" s="1" t="s">
+      <c r="L65" s="1" t="s">
         <v>658</v>
       </c>
-      <c r="L65" s="1" t="s">
+      <c r="M65" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M65" t="s">
-        <v>788</v>
-      </c>
-      <c r="N65" s="5" t="s">
+      <c r="N65" t="s">
+        <v>788</v>
+      </c>
+      <c r="O65" s="5" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="96" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -5810,26 +6340,29 @@
       <c r="H66" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="I66" s="4" t="s">
+      <c r="I66" t="s">
+        <v>921</v>
+      </c>
+      <c r="J66" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="J66" s="1" t="s">
+      <c r="K66" s="1" t="s">
         <v>660</v>
       </c>
-      <c r="K66" s="1" t="s">
+      <c r="L66" s="1" t="s">
         <v>661</v>
       </c>
-      <c r="L66" s="1" t="s">
+      <c r="M66" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M66" t="s">
-        <v>788</v>
-      </c>
-      <c r="N66" s="5" t="s">
+      <c r="N66" t="s">
+        <v>788</v>
+      </c>
+      <c r="O66" s="5" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -5854,26 +6387,29 @@
       <c r="H67" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="I67" s="4" t="s">
+      <c r="I67" t="s">
+        <v>922</v>
+      </c>
+      <c r="J67" s="4" t="s">
         <v>662</v>
       </c>
-      <c r="J67" s="1" t="s">
+      <c r="K67" s="1" t="s">
         <v>663</v>
       </c>
-      <c r="K67" s="1" t="s">
+      <c r="L67" s="1" t="s">
         <v>664</v>
       </c>
-      <c r="L67" s="1" t="s">
+      <c r="M67" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M67" t="s">
-        <v>788</v>
-      </c>
-      <c r="N67" s="5" t="s">
+      <c r="N67" t="s">
+        <v>788</v>
+      </c>
+      <c r="O67" s="5" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -5895,26 +6431,29 @@
       <c r="H68" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="I68" s="4" t="s">
+      <c r="I68" t="s">
+        <v>923</v>
+      </c>
+      <c r="J68" s="4" t="s">
         <v>665</v>
       </c>
-      <c r="J68" s="1" t="s">
+      <c r="K68" s="1" t="s">
         <v>666</v>
       </c>
-      <c r="K68" s="1" t="s">
+      <c r="L68" s="1" t="s">
         <v>667</v>
       </c>
-      <c r="L68" s="1" t="s">
+      <c r="M68" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M68" t="s">
-        <v>788</v>
-      </c>
-      <c r="N68" s="5" t="s">
+      <c r="N68" t="s">
+        <v>788</v>
+      </c>
+      <c r="O68" s="5" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -5936,26 +6475,29 @@
       <c r="H69" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="I69" s="4" t="s">
+      <c r="I69" t="s">
+        <v>924</v>
+      </c>
+      <c r="J69" s="4" t="s">
         <v>668</v>
       </c>
-      <c r="J69" s="1" t="s">
+      <c r="K69" s="1" t="s">
         <v>669</v>
       </c>
-      <c r="K69" s="1" t="s">
+      <c r="L69" s="1" t="s">
         <v>670</v>
       </c>
-      <c r="L69" s="1" t="s">
+      <c r="M69" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M69" t="s">
-        <v>788</v>
-      </c>
-      <c r="N69" s="5" t="s">
+      <c r="N69" t="s">
+        <v>788</v>
+      </c>
+      <c r="O69" s="5" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -5977,26 +6519,29 @@
       <c r="H70" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="I70" s="4" t="s">
+      <c r="I70" t="s">
+        <v>925</v>
+      </c>
+      <c r="J70" s="4" t="s">
         <v>671</v>
       </c>
-      <c r="J70" s="1" t="s">
+      <c r="K70" s="1" t="s">
         <v>672</v>
       </c>
-      <c r="K70" s="1" t="s">
+      <c r="L70" s="1" t="s">
         <v>673</v>
       </c>
-      <c r="L70" s="1" t="s">
+      <c r="M70" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M70" t="s">
-        <v>788</v>
-      </c>
-      <c r="N70" s="5" t="s">
+      <c r="N70" t="s">
+        <v>788</v>
+      </c>
+      <c r="O70" s="5" t="s">
         <v>798</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -6018,26 +6563,29 @@
       <c r="H71" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="I71" s="4" t="s">
+      <c r="I71" t="s">
+        <v>926</v>
+      </c>
+      <c r="J71" s="4" t="s">
         <v>674</v>
       </c>
-      <c r="J71" s="1" t="s">
+      <c r="K71" s="1" t="s">
         <v>675</v>
       </c>
-      <c r="K71" s="1" t="s">
+      <c r="L71" s="1" t="s">
         <v>676</v>
       </c>
-      <c r="L71" s="1" t="s">
+      <c r="M71" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M71" t="s">
-        <v>788</v>
-      </c>
-      <c r="N71" s="5" t="s">
+      <c r="N71" t="s">
+        <v>788</v>
+      </c>
+      <c r="O71" s="5" t="s">
         <v>798</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -6062,26 +6610,29 @@
       <c r="H72" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="I72" s="4" t="s">
+      <c r="I72" t="s">
+        <v>927</v>
+      </c>
+      <c r="J72" s="4" t="s">
         <v>677</v>
       </c>
-      <c r="J72" s="4" t="s">
+      <c r="K72" s="4" t="s">
         <v>848</v>
       </c>
-      <c r="K72" s="1" t="s">
+      <c r="L72" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="L72" s="1" t="s">
+      <c r="M72" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M72" t="s">
-        <v>788</v>
-      </c>
-      <c r="N72" s="5" t="s">
+      <c r="N72" t="s">
+        <v>788</v>
+      </c>
+      <c r="O72" s="5" t="s">
         <v>798</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -6106,26 +6657,29 @@
       <c r="H73" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="I73" s="4" t="s">
+      <c r="I73" t="s">
+        <v>928</v>
+      </c>
+      <c r="J73" s="4" t="s">
         <v>679</v>
       </c>
-      <c r="J73" s="4" t="s">
+      <c r="K73" s="4" t="s">
         <v>849</v>
       </c>
-      <c r="K73" s="1" t="s">
+      <c r="L73" s="1" t="s">
         <v>680</v>
       </c>
-      <c r="L73" s="1" t="s">
+      <c r="M73" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M73" t="s">
-        <v>788</v>
-      </c>
-      <c r="N73" s="5" t="s">
+      <c r="N73" t="s">
+        <v>788</v>
+      </c>
+      <c r="O73" s="5" t="s">
         <v>798</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -6150,26 +6704,29 @@
       <c r="H74" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="I74" s="4" t="s">
+      <c r="I74" t="s">
+        <v>929</v>
+      </c>
+      <c r="J74" s="4" t="s">
         <v>681</v>
       </c>
-      <c r="J74" s="4" t="s">
+      <c r="K74" s="4" t="s">
         <v>850</v>
       </c>
-      <c r="K74" s="1" t="s">
+      <c r="L74" s="1" t="s">
         <v>682</v>
       </c>
-      <c r="L74" s="1" t="s">
+      <c r="M74" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M74" t="s">
-        <v>788</v>
-      </c>
-      <c r="N74" s="5" t="s">
+      <c r="N74" t="s">
+        <v>788</v>
+      </c>
+      <c r="O74" s="5" t="s">
         <v>798</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -6191,26 +6748,29 @@
       <c r="H75" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="I75" s="4" t="s">
+      <c r="I75" t="s">
+        <v>930</v>
+      </c>
+      <c r="J75" s="4" t="s">
         <v>683</v>
       </c>
-      <c r="J75" s="4" t="s">
+      <c r="K75" s="4" t="s">
         <v>851</v>
       </c>
-      <c r="K75" s="1" t="s">
+      <c r="L75" s="1" t="s">
         <v>684</v>
       </c>
-      <c r="L75" s="1" t="s">
+      <c r="M75" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M75" t="s">
-        <v>788</v>
-      </c>
-      <c r="N75" s="5" t="s">
+      <c r="N75" t="s">
+        <v>788</v>
+      </c>
+      <c r="O75" s="5" t="s">
         <v>798</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -6232,26 +6792,29 @@
       <c r="H76" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="I76" s="4" t="s">
+      <c r="I76" t="s">
+        <v>931</v>
+      </c>
+      <c r="J76" s="4" t="s">
         <v>685</v>
       </c>
-      <c r="J76" s="4" t="s">
+      <c r="K76" s="4" t="s">
         <v>852</v>
       </c>
-      <c r="K76" s="1" t="s">
+      <c r="L76" s="1" t="s">
         <v>686</v>
       </c>
-      <c r="L76" s="1" t="s">
+      <c r="M76" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M76" t="s">
-        <v>788</v>
-      </c>
-      <c r="N76" s="5" t="s">
+      <c r="N76" t="s">
+        <v>788</v>
+      </c>
+      <c r="O76" s="5" t="s">
         <v>798</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -6276,26 +6839,29 @@
       <c r="H77" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="I77" s="4" t="s">
+      <c r="I77" t="s">
+        <v>932</v>
+      </c>
+      <c r="J77" s="4" t="s">
         <v>687</v>
       </c>
-      <c r="J77" s="1" t="s">
+      <c r="K77" s="1" t="s">
         <v>688</v>
       </c>
-      <c r="K77" s="1" t="s">
+      <c r="L77" s="1" t="s">
         <v>689</v>
       </c>
-      <c r="L77" s="1" t="s">
+      <c r="M77" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M77" t="s">
-        <v>788</v>
-      </c>
-      <c r="N77" s="5" t="s">
+      <c r="N77" t="s">
+        <v>788</v>
+      </c>
+      <c r="O77" s="5" t="s">
         <v>799</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -6320,26 +6886,29 @@
       <c r="H78" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="I78" s="4" t="s">
+      <c r="I78" t="s">
+        <v>933</v>
+      </c>
+      <c r="J78" s="4" t="s">
         <v>690</v>
       </c>
-      <c r="J78" s="1" t="s">
+      <c r="K78" s="1" t="s">
         <v>691</v>
       </c>
-      <c r="K78" s="1" t="s">
+      <c r="L78" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="L78" s="1" t="s">
+      <c r="M78" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M78" t="s">
-        <v>788</v>
-      </c>
-      <c r="N78" s="5" t="s">
+      <c r="N78" t="s">
+        <v>788</v>
+      </c>
+      <c r="O78" s="5" t="s">
         <v>799</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -6361,26 +6930,29 @@
       <c r="H79" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="I79" s="4" t="s">
+      <c r="I79" t="s">
+        <v>934</v>
+      </c>
+      <c r="J79" s="4" t="s">
         <v>693</v>
       </c>
-      <c r="J79" s="1" t="s">
+      <c r="K79" s="1" t="s">
         <v>694</v>
       </c>
-      <c r="K79" s="1" t="s">
+      <c r="L79" s="1" t="s">
         <v>695</v>
       </c>
-      <c r="L79" s="1" t="s">
+      <c r="M79" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M79" t="s">
-        <v>788</v>
-      </c>
-      <c r="N79" s="5" t="s">
+      <c r="N79" t="s">
+        <v>788</v>
+      </c>
+      <c r="O79" s="5" t="s">
         <v>799</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -6405,26 +6977,29 @@
       <c r="H80" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="I80" s="4" t="s">
+      <c r="I80" t="s">
+        <v>935</v>
+      </c>
+      <c r="J80" s="4" t="s">
         <v>696</v>
       </c>
-      <c r="J80" s="1" t="s">
+      <c r="K80" s="1" t="s">
         <v>697</v>
       </c>
-      <c r="K80" s="1" t="s">
+      <c r="L80" s="1" t="s">
         <v>698</v>
       </c>
-      <c r="L80" s="1" t="s">
+      <c r="M80" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M80" t="s">
-        <v>788</v>
-      </c>
-      <c r="N80" s="5" t="s">
+      <c r="N80" t="s">
+        <v>788</v>
+      </c>
+      <c r="O80" s="5" t="s">
         <v>799</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -6446,26 +7021,29 @@
       <c r="H81" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="I81" s="4" t="s">
+      <c r="I81" t="s">
+        <v>936</v>
+      </c>
+      <c r="J81" s="4" t="s">
         <v>699</v>
       </c>
-      <c r="J81" s="1" t="s">
+      <c r="K81" s="1" t="s">
         <v>700</v>
       </c>
-      <c r="K81" s="1" t="s">
+      <c r="L81" s="1" t="s">
         <v>701</v>
       </c>
-      <c r="L81" s="1" t="s">
+      <c r="M81" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M81" t="s">
-        <v>788</v>
-      </c>
-      <c r="N81" s="5" t="s">
+      <c r="N81" t="s">
+        <v>788</v>
+      </c>
+      <c r="O81" s="5" t="s">
         <v>799</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -6487,26 +7065,29 @@
       <c r="H82" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="I82" s="4" t="s">
+      <c r="I82" t="s">
+        <v>937</v>
+      </c>
+      <c r="J82" s="4" t="s">
         <v>702</v>
       </c>
-      <c r="J82" s="1" t="s">
+      <c r="K82" s="1" t="s">
         <v>703</v>
       </c>
-      <c r="K82" s="1" t="s">
+      <c r="L82" s="1" t="s">
         <v>704</v>
       </c>
-      <c r="L82" s="1" t="s">
+      <c r="M82" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M82" t="s">
-        <v>788</v>
-      </c>
-      <c r="N82" s="5" t="s">
+      <c r="N82" t="s">
+        <v>788</v>
+      </c>
+      <c r="O82" s="5" t="s">
         <v>799</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -6531,26 +7112,29 @@
       <c r="H83" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="I83" s="4" t="s">
+      <c r="I83" t="s">
+        <v>938</v>
+      </c>
+      <c r="J83" s="4" t="s">
         <v>705</v>
       </c>
-      <c r="J83" s="1" t="s">
+      <c r="K83" s="1" t="s">
         <v>706</v>
       </c>
-      <c r="K83" s="1" t="s">
+      <c r="L83" s="1" t="s">
         <v>707</v>
       </c>
-      <c r="L83" s="1" t="s">
+      <c r="M83" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="M83" t="s">
-        <v>788</v>
-      </c>
-      <c r="N83" s="5" t="s">
+      <c r="N83" t="s">
+        <v>788</v>
+      </c>
+      <c r="O83" s="5" t="s">
         <v>800</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -6575,26 +7159,29 @@
       <c r="H84" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="I84" s="4" t="s">
+      <c r="I84" t="s">
+        <v>939</v>
+      </c>
+      <c r="J84" s="4" t="s">
         <v>708</v>
       </c>
-      <c r="J84" s="1" t="s">
+      <c r="K84" s="1" t="s">
         <v>709</v>
       </c>
-      <c r="K84" s="1" t="s">
+      <c r="L84" s="1" t="s">
         <v>710</v>
       </c>
-      <c r="L84" s="1" t="s">
+      <c r="M84" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="M84" t="s">
-        <v>788</v>
-      </c>
-      <c r="N84" s="5" t="s">
+      <c r="N84" t="s">
+        <v>788</v>
+      </c>
+      <c r="O84" s="5" t="s">
         <v>800</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -6619,26 +7206,29 @@
       <c r="H85" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="I85" s="4" t="s">
+      <c r="I85" t="s">
+        <v>940</v>
+      </c>
+      <c r="J85" s="4" t="s">
         <v>711</v>
       </c>
-      <c r="J85" s="1" t="s">
+      <c r="K85" s="1" t="s">
         <v>712</v>
       </c>
-      <c r="K85" s="1" t="s">
+      <c r="L85" s="1" t="s">
         <v>713</v>
       </c>
-      <c r="L85" s="1" t="s">
+      <c r="M85" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="M85" t="s">
-        <v>788</v>
-      </c>
-      <c r="N85" s="5" t="s">
+      <c r="N85" t="s">
+        <v>788</v>
+      </c>
+      <c r="O85" s="5" t="s">
         <v>800</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -6663,26 +7253,29 @@
       <c r="H86" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="I86" s="4" t="s">
+      <c r="I86" t="s">
+        <v>941</v>
+      </c>
+      <c r="J86" s="4" t="s">
         <v>714</v>
       </c>
-      <c r="J86" s="1" t="s">
+      <c r="K86" s="1" t="s">
         <v>715</v>
       </c>
-      <c r="K86" s="1" t="s">
+      <c r="L86" s="1" t="s">
         <v>716</v>
       </c>
-      <c r="L86" s="1" t="s">
+      <c r="M86" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="M86" t="s">
-        <v>788</v>
-      </c>
-      <c r="N86" s="5" t="s">
+      <c r="N86" t="s">
+        <v>788</v>
+      </c>
+      <c r="O86" s="5" t="s">
         <v>800</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -6707,26 +7300,29 @@
       <c r="H87" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="I87" s="4" t="s">
+      <c r="I87" t="s">
+        <v>942</v>
+      </c>
+      <c r="J87" s="4" t="s">
         <v>717</v>
       </c>
-      <c r="J87" s="1" t="s">
+      <c r="K87" s="1" t="s">
         <v>718</v>
       </c>
-      <c r="K87" s="1" t="s">
+      <c r="L87" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="L87" s="1" t="s">
+      <c r="M87" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="M87" t="s">
-        <v>788</v>
-      </c>
-      <c r="N87" s="5" t="s">
+      <c r="N87" t="s">
+        <v>788</v>
+      </c>
+      <c r="O87" s="5" t="s">
         <v>800</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -6748,26 +7344,29 @@
       <c r="H88" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="I88" s="4" t="s">
+      <c r="I88" t="s">
+        <v>943</v>
+      </c>
+      <c r="J88" s="4" t="s">
         <v>720</v>
       </c>
-      <c r="J88" s="1" t="s">
+      <c r="K88" s="1" t="s">
         <v>721</v>
       </c>
-      <c r="K88" s="1" t="s">
+      <c r="L88" s="1" t="s">
         <v>722</v>
       </c>
-      <c r="L88" s="1" t="s">
+      <c r="M88" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="M88" t="s">
-        <v>788</v>
-      </c>
-      <c r="N88" s="5" t="s">
+      <c r="N88" t="s">
+        <v>788</v>
+      </c>
+      <c r="O88" s="5" t="s">
         <v>800</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -6792,26 +7391,29 @@
       <c r="H89" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="I89" s="4" t="s">
+      <c r="I89" t="s">
+        <v>944</v>
+      </c>
+      <c r="J89" s="4" t="s">
         <v>723</v>
       </c>
-      <c r="J89" s="4" t="s">
+      <c r="K89" s="4" t="s">
         <v>853</v>
       </c>
-      <c r="K89" s="1" t="s">
+      <c r="L89" s="1" t="s">
         <v>724</v>
       </c>
-      <c r="L89" s="1" t="s">
+      <c r="M89" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="M89" t="s">
-        <v>788</v>
-      </c>
-      <c r="N89" s="5" t="s">
+      <c r="N89" t="s">
+        <v>788</v>
+      </c>
+      <c r="O89" s="5" t="s">
         <v>800</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -6833,26 +7435,29 @@
       <c r="H90" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="I90" s="4" t="s">
+      <c r="I90" t="s">
+        <v>945</v>
+      </c>
+      <c r="J90" s="4" t="s">
         <v>725</v>
       </c>
-      <c r="J90" s="4" t="s">
+      <c r="K90" s="4" t="s">
         <v>854</v>
       </c>
-      <c r="K90" s="1" t="s">
+      <c r="L90" s="1" t="s">
         <v>726</v>
       </c>
-      <c r="L90" s="1" t="s">
+      <c r="M90" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="M90" t="s">
-        <v>788</v>
-      </c>
-      <c r="N90" s="5" t="s">
+      <c r="N90" t="s">
+        <v>788</v>
+      </c>
+      <c r="O90" s="5" t="s">
         <v>800</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -6874,26 +7479,29 @@
       <c r="H91" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="I91" s="4" t="s">
+      <c r="I91" t="s">
+        <v>946</v>
+      </c>
+      <c r="J91" s="4" t="s">
         <v>727</v>
       </c>
-      <c r="J91" s="4" t="s">
+      <c r="K91" s="4" t="s">
         <v>855</v>
       </c>
-      <c r="K91" s="1" t="s">
+      <c r="L91" s="1" t="s">
         <v>728</v>
       </c>
-      <c r="L91" s="1" t="s">
+      <c r="M91" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="M91" t="s">
-        <v>788</v>
-      </c>
-      <c r="N91" s="5" t="s">
+      <c r="N91" t="s">
+        <v>788</v>
+      </c>
+      <c r="O91" s="5" t="s">
         <v>800</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -6915,26 +7523,29 @@
       <c r="H92" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="I92" s="4" t="s">
+      <c r="I92" t="s">
+        <v>947</v>
+      </c>
+      <c r="J92" s="4" t="s">
         <v>729</v>
       </c>
-      <c r="J92" s="1" t="s">
+      <c r="K92" s="1" t="s">
         <v>730</v>
       </c>
-      <c r="K92" s="1" t="s">
+      <c r="L92" s="1" t="s">
         <v>731</v>
       </c>
-      <c r="L92" s="1" t="s">
+      <c r="M92" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M92" t="s">
-        <v>788</v>
-      </c>
-      <c r="N92" s="5" t="s">
+      <c r="N92" t="s">
+        <v>788</v>
+      </c>
+      <c r="O92" s="5" t="s">
         <v>801</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -6956,26 +7567,29 @@
       <c r="H93" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="I93" s="4" t="s">
+      <c r="I93" t="s">
+        <v>948</v>
+      </c>
+      <c r="J93" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="J93" s="1" t="s">
+      <c r="K93" s="1" t="s">
         <v>733</v>
       </c>
-      <c r="K93" s="1" t="s">
+      <c r="L93" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="L93" s="1" t="s">
+      <c r="M93" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M93" t="s">
-        <v>788</v>
-      </c>
-      <c r="N93" s="5" t="s">
+      <c r="N93" t="s">
+        <v>788</v>
+      </c>
+      <c r="O93" s="5" t="s">
         <v>801</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -6994,26 +7608,29 @@
       <c r="H94" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="I94" s="4" t="s">
+      <c r="I94" t="s">
+        <v>949</v>
+      </c>
+      <c r="J94" s="4" t="s">
         <v>735</v>
       </c>
-      <c r="J94" s="1" t="s">
+      <c r="K94" s="1" t="s">
         <v>736</v>
       </c>
-      <c r="K94" s="1" t="s">
+      <c r="L94" s="1" t="s">
         <v>737</v>
       </c>
-      <c r="L94" s="1" t="s">
+      <c r="M94" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M94" t="s">
-        <v>788</v>
-      </c>
-      <c r="N94" s="5" t="s">
+      <c r="N94" t="s">
+        <v>788</v>
+      </c>
+      <c r="O94" s="5" t="s">
         <v>801</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -7038,26 +7655,29 @@
       <c r="H95" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="I95" s="4" t="s">
+      <c r="I95" t="s">
+        <v>950</v>
+      </c>
+      <c r="J95" s="4" t="s">
         <v>738</v>
       </c>
-      <c r="J95" s="1" t="s">
+      <c r="K95" s="1" t="s">
         <v>739</v>
       </c>
-      <c r="K95" s="1" t="s">
+      <c r="L95" s="1" t="s">
         <v>740</v>
       </c>
-      <c r="L95" s="1" t="s">
+      <c r="M95" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M95" t="s">
-        <v>788</v>
-      </c>
-      <c r="N95" s="5" t="s">
+      <c r="N95" t="s">
+        <v>788</v>
+      </c>
+      <c r="O95" s="5" t="s">
         <v>801</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -7079,26 +7699,29 @@
       <c r="H96" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="I96" s="4" t="s">
+      <c r="I96" t="s">
+        <v>951</v>
+      </c>
+      <c r="J96" s="4" t="s">
         <v>741</v>
       </c>
-      <c r="J96" s="1" t="s">
+      <c r="K96" s="1" t="s">
         <v>742</v>
       </c>
-      <c r="K96" s="1" t="s">
+      <c r="L96" s="1" t="s">
         <v>743</v>
       </c>
-      <c r="L96" s="1" t="s">
+      <c r="M96" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M96" t="s">
-        <v>788</v>
-      </c>
-      <c r="N96" s="5" t="s">
+      <c r="N96" t="s">
+        <v>788</v>
+      </c>
+      <c r="O96" s="5" t="s">
         <v>801</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -7123,26 +7746,29 @@
       <c r="H97" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="I97" s="4" t="s">
+      <c r="I97" t="s">
+        <v>952</v>
+      </c>
+      <c r="J97" s="4" t="s">
         <v>744</v>
       </c>
-      <c r="J97" s="1" t="s">
+      <c r="K97" s="1" t="s">
         <v>745</v>
       </c>
-      <c r="K97" s="1" t="s">
+      <c r="L97" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="L97" s="1" t="s">
+      <c r="M97" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M97" t="s">
-        <v>788</v>
-      </c>
-      <c r="N97" s="5" t="s">
+      <c r="N97" t="s">
+        <v>788</v>
+      </c>
+      <c r="O97" s="5" t="s">
         <v>801</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -7164,26 +7790,29 @@
       <c r="H98" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="I98" s="4" t="s">
+      <c r="I98" t="s">
+        <v>953</v>
+      </c>
+      <c r="J98" s="4" t="s">
         <v>747</v>
       </c>
-      <c r="J98" s="1" t="s">
+      <c r="K98" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="K98" s="1" t="s">
+      <c r="L98" s="1" t="s">
         <v>749</v>
       </c>
-      <c r="L98" s="1" t="s">
+      <c r="M98" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M98" t="s">
-        <v>788</v>
-      </c>
-      <c r="N98" s="5" t="s">
+      <c r="N98" t="s">
+        <v>788</v>
+      </c>
+      <c r="O98" s="5" t="s">
         <v>801</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -7205,26 +7834,29 @@
       <c r="H99" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="I99" s="4" t="s">
+      <c r="I99" t="s">
+        <v>954</v>
+      </c>
+      <c r="J99" s="4" t="s">
         <v>750</v>
       </c>
-      <c r="J99" s="1" t="s">
+      <c r="K99" s="1" t="s">
         <v>751</v>
       </c>
-      <c r="K99" s="1" t="s">
+      <c r="L99" s="1" t="s">
         <v>752</v>
       </c>
-      <c r="L99" s="1" t="s">
+      <c r="M99" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M99" t="s">
-        <v>788</v>
-      </c>
-      <c r="N99" s="5" t="s">
+      <c r="N99" t="s">
+        <v>788</v>
+      </c>
+      <c r="O99" s="5" t="s">
         <v>801</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -7246,26 +7878,29 @@
       <c r="H100" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="I100" s="4" t="s">
+      <c r="I100" t="s">
+        <v>955</v>
+      </c>
+      <c r="J100" s="4" t="s">
         <v>753</v>
       </c>
-      <c r="J100" s="1" t="s">
+      <c r="K100" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="K100" s="1" t="s">
+      <c r="L100" s="1" t="s">
         <v>755</v>
       </c>
-      <c r="L100" s="1" t="s">
+      <c r="M100" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="M100" t="s">
-        <v>788</v>
-      </c>
-      <c r="N100" s="5" t="s">
+      <c r="N100" t="s">
+        <v>788</v>
+      </c>
+      <c r="O100" s="5" t="s">
         <v>801</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -7287,26 +7922,29 @@
       <c r="H101" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="I101" s="4" t="s">
+      <c r="I101" t="s">
+        <v>956</v>
+      </c>
+      <c r="J101" s="4" t="s">
         <v>756</v>
       </c>
-      <c r="J101" s="1" t="s">
+      <c r="K101" s="1" t="s">
         <v>757</v>
       </c>
-      <c r="K101" s="1" t="s">
+      <c r="L101" s="1" t="s">
         <v>758</v>
       </c>
-      <c r="L101" s="1" t="s">
+      <c r="M101" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="M101" t="s">
-        <v>788</v>
-      </c>
-      <c r="N101" s="5" t="s">
+      <c r="N101" t="s">
+        <v>788</v>
+      </c>
+      <c r="O101" s="5" t="s">
         <v>802</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -7331,26 +7969,29 @@
       <c r="H102" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="I102" s="4" t="s">
+      <c r="I102" t="s">
+        <v>957</v>
+      </c>
+      <c r="J102" s="4" t="s">
         <v>759</v>
       </c>
-      <c r="J102" s="1" t="s">
+      <c r="K102" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="K102" s="1" t="s">
+      <c r="L102" s="1" t="s">
         <v>761</v>
       </c>
-      <c r="L102" s="1" t="s">
+      <c r="M102" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="M102" t="s">
-        <v>788</v>
-      </c>
-      <c r="N102" s="6" t="s">
+      <c r="N102" t="s">
+        <v>788</v>
+      </c>
+      <c r="O102" s="6" t="s">
         <v>802</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -7372,26 +8013,29 @@
       <c r="H103" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="I103" s="4" t="s">
+      <c r="I103" t="s">
+        <v>958</v>
+      </c>
+      <c r="J103" s="4" t="s">
         <v>762</v>
       </c>
-      <c r="J103" s="1" t="s">
+      <c r="K103" s="1" t="s">
         <v>763</v>
       </c>
-      <c r="K103" s="1" t="s">
+      <c r="L103" s="1" t="s">
         <v>764</v>
       </c>
-      <c r="L103" s="1" t="s">
+      <c r="M103" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="M103" t="s">
-        <v>788</v>
-      </c>
-      <c r="N103" s="6" t="s">
+      <c r="N103" t="s">
+        <v>788</v>
+      </c>
+      <c r="O103" s="6" t="s">
         <v>802</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -7416,26 +8060,29 @@
       <c r="H104" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="I104" s="4" t="s">
+      <c r="I104" t="s">
+        <v>959</v>
+      </c>
+      <c r="J104" s="4" t="s">
         <v>765</v>
       </c>
-      <c r="J104" s="1" t="s">
+      <c r="K104" s="1" t="s">
         <v>766</v>
       </c>
-      <c r="K104" s="1" t="s">
+      <c r="L104" s="1" t="s">
         <v>767</v>
       </c>
-      <c r="L104" s="1" t="s">
+      <c r="M104" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="M104" t="s">
-        <v>788</v>
-      </c>
-      <c r="N104" s="6" t="s">
+      <c r="N104" t="s">
+        <v>788</v>
+      </c>
+      <c r="O104" s="6" t="s">
         <v>802</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -7457,26 +8104,29 @@
       <c r="H105" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="I105" s="4" t="s">
+      <c r="I105" t="s">
+        <v>960</v>
+      </c>
+      <c r="J105" s="4" t="s">
         <v>768</v>
       </c>
-      <c r="J105" s="4" t="s">
+      <c r="K105" s="4" t="s">
         <v>808</v>
       </c>
-      <c r="K105" s="1" t="s">
+      <c r="L105" s="1" t="s">
         <v>769</v>
       </c>
-      <c r="L105" s="1" t="s">
+      <c r="M105" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="M105" t="s">
-        <v>788</v>
-      </c>
-      <c r="N105" s="6" t="s">
+      <c r="N105" t="s">
+        <v>788</v>
+      </c>
+      <c r="O105" s="6" t="s">
         <v>802</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -7501,26 +8151,29 @@
       <c r="H106" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="I106" s="4" t="s">
+      <c r="I106" t="s">
+        <v>961</v>
+      </c>
+      <c r="J106" s="4" t="s">
         <v>770</v>
       </c>
-      <c r="J106" s="4" t="s">
+      <c r="K106" s="4" t="s">
         <v>809</v>
       </c>
-      <c r="K106" s="1" t="s">
+      <c r="L106" s="1" t="s">
         <v>771</v>
       </c>
-      <c r="L106" s="1" t="s">
+      <c r="M106" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="M106" t="s">
-        <v>788</v>
-      </c>
-      <c r="N106" s="6" t="s">
+      <c r="N106" t="s">
+        <v>788</v>
+      </c>
+      <c r="O106" s="6" t="s">
         <v>802</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -7542,26 +8195,29 @@
       <c r="H107" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="I107" s="4" t="s">
+      <c r="I107" t="s">
+        <v>962</v>
+      </c>
+      <c r="J107" s="4" t="s">
         <v>772</v>
       </c>
-      <c r="J107" s="1" t="s">
+      <c r="K107" s="1" t="s">
         <v>773</v>
       </c>
-      <c r="K107" s="1" t="s">
+      <c r="L107" s="1" t="s">
         <v>774</v>
       </c>
-      <c r="L107" s="1" t="s">
+      <c r="M107" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="M107" t="s">
-        <v>788</v>
-      </c>
-      <c r="N107" s="6" t="s">
+      <c r="N107" t="s">
+        <v>788</v>
+      </c>
+      <c r="O107" s="6" t="s">
         <v>802</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -7583,26 +8239,29 @@
       <c r="H108" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="I108" s="4" t="s">
+      <c r="I108" t="s">
+        <v>963</v>
+      </c>
+      <c r="J108" s="4" t="s">
         <v>775</v>
       </c>
-      <c r="J108" s="1" t="s">
+      <c r="K108" s="1" t="s">
         <v>776</v>
       </c>
-      <c r="K108" s="1" t="s">
+      <c r="L108" s="1" t="s">
         <v>777</v>
       </c>
-      <c r="L108" s="1" t="s">
+      <c r="M108" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="M108" t="s">
-        <v>788</v>
-      </c>
-      <c r="N108" s="6" t="s">
+      <c r="N108" t="s">
+        <v>788</v>
+      </c>
+      <c r="O108" s="6" t="s">
         <v>802</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -7624,26 +8283,29 @@
       <c r="H109" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="I109" s="4" t="s">
+      <c r="I109" t="s">
+        <v>964</v>
+      </c>
+      <c r="J109" s="4" t="s">
         <v>778</v>
       </c>
-      <c r="J109" s="1" t="s">
+      <c r="K109" s="1" t="s">
         <v>779</v>
       </c>
-      <c r="K109" s="1" t="s">
+      <c r="L109" s="1" t="s">
         <v>780</v>
       </c>
-      <c r="L109" s="1" t="s">
+      <c r="M109" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="M109" t="s">
-        <v>788</v>
-      </c>
-      <c r="N109" s="6" t="s">
+      <c r="N109" t="s">
+        <v>788</v>
+      </c>
+      <c r="O109" s="6" t="s">
         <v>802</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -7668,26 +8330,29 @@
       <c r="H110" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="I110" s="4" t="s">
+      <c r="I110" t="s">
+        <v>965</v>
+      </c>
+      <c r="J110" s="4" t="s">
         <v>781</v>
       </c>
-      <c r="J110" s="1" t="s">
+      <c r="K110" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="K110" s="1" t="s">
+      <c r="L110" s="1" t="s">
         <v>783</v>
       </c>
-      <c r="L110" s="1" t="s">
+      <c r="M110" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="M110" t="s">
-        <v>788</v>
-      </c>
-      <c r="N110" s="6" t="s">
+      <c r="N110" t="s">
+        <v>788</v>
+      </c>
+      <c r="O110" s="6" t="s">
         <v>802</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -7709,53 +8374,56 @@
       <c r="H111" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="I111" s="4" t="s">
+      <c r="I111" t="s">
+        <v>966</v>
+      </c>
+      <c r="J111" s="4" t="s">
         <v>784</v>
       </c>
-      <c r="J111" s="1" t="s">
+      <c r="K111" s="1" t="s">
         <v>785</v>
       </c>
-      <c r="K111" s="1" t="s">
+      <c r="L111" s="1" t="s">
         <v>786</v>
       </c>
-      <c r="L111" s="1" t="s">
+      <c r="M111" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="M111" t="s">
-        <v>788</v>
-      </c>
-      <c r="N111" s="6" t="s">
+      <c r="N111" t="s">
+        <v>788</v>
+      </c>
+      <c r="O111" s="6" t="s">
         <v>802</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N10" r:id="rId1" xr:uid="{8D2C38B8-FFB6-5E49-9C32-FD70F8BF5C70}"/>
-    <hyperlink ref="N11:N17" r:id="rId2" display="https://archive.org/download/gri_c00033125012743312/gri_c00033125012743312_jp2.zip/gri_c00033125012743312_jp2%2Fgri_c00033125012743312_0033.jpg" xr:uid="{CB684880-C13B-A948-B28B-D0F22E6D61DB}"/>
-    <hyperlink ref="N18" r:id="rId3" xr:uid="{3D2A0FB2-ABE1-0849-80C3-D3CD01B0995F}"/>
-    <hyperlink ref="N19:N24" r:id="rId4" display="https://archive.org/download/gri_c00033125012743312/gri_c00033125012743312_jp2.zip/gri_c00033125012743312_jp2%2Fgri_c00033125012743312_0037.jpg" xr:uid="{0D5118B9-BCC7-3146-A3F3-B5576F2C73D3}"/>
-    <hyperlink ref="N25" r:id="rId5" xr:uid="{DEBB1F8F-01AA-1446-B6AD-CEEDB824B545}"/>
-    <hyperlink ref="N26:N35" r:id="rId6" display="https://archive.org/download/gri_c00033125012743312/gri_c00033125012743312_jp2.zip/gri_c00033125012743312_jp2%2Fgri_c00033125012743312_0041.jpg" xr:uid="{F31D613A-AAF3-5F4F-BE00-BC67B616D348}"/>
-    <hyperlink ref="N36" r:id="rId7" xr:uid="{A965DEFD-E821-B747-8F47-763DB6CFCDA5}"/>
-    <hyperlink ref="N37:N45" r:id="rId8" display="https://archive.org/download/gri_c00033125012743312/gri_c00033125012743312_jp2.zip/gri_c00033125012743312_jp2%2Fgri_c00033125012743312_0045.jpg" xr:uid="{90FBAD6C-4314-4648-999A-9318848CD478}"/>
-    <hyperlink ref="N46" r:id="rId9" xr:uid="{F38B3821-6B78-8245-AA5F-A171E6732863}"/>
-    <hyperlink ref="N47" r:id="rId10" xr:uid="{1145454B-D921-BA4D-A02B-1249ECB515EB}"/>
-    <hyperlink ref="N48:N54" r:id="rId11" display="https://archive.org/download/gri_c00033125012743312/gri_c00033125012743312_jp2.zip/gri_c00033125012743312_jp2%2Fgri_c00033125012743312_0049.jpg" xr:uid="{68184C3E-4B1F-1642-9D16-DA249976B264}"/>
-    <hyperlink ref="N55" r:id="rId12" xr:uid="{900CB1B8-822D-2B46-A8F0-8E6E907F177D}"/>
-    <hyperlink ref="N56:N62" r:id="rId13" display="https://archive.org/download/gri_c00033125012743312/gri_c00033125012743312_jp2.zip/gri_c00033125012743312_jp2%2Fgri_c00033125012743312_0052.jpg" xr:uid="{14CEA8D5-83CC-1D48-8FFA-2BE840D0DEAD}"/>
-    <hyperlink ref="N63" r:id="rId14" xr:uid="{B8EDAC7D-15E7-B44C-8207-76FC3D6F981C}"/>
-    <hyperlink ref="N64:N68" r:id="rId15" display="https://archive.org/download/gri_c00033125012743312/gri_c00033125012743312_jp2.zip/gri_c00033125012743312_jp2%2Fgri_c00033125012743312_0056.jpg" xr:uid="{747F0C47-4978-3A42-ADEC-D041490CFC3A}"/>
-    <hyperlink ref="N69" r:id="rId16" xr:uid="{53230F16-35CB-ED46-AE27-7C0C06930D06}"/>
-    <hyperlink ref="N70" r:id="rId17" xr:uid="{144055C7-22F3-0F40-844D-D61E3E061E70}"/>
-    <hyperlink ref="N71:N75" r:id="rId18" display="https://archive.org/download/gri_c00033125012743312/gri_c00033125012743312_jp2.zip/gri_c00033125012743312_jp2%2Fgri_c00033125012743312_0059.jpg" xr:uid="{A477BA26-9910-4646-AECB-B39F82D546EC}"/>
-    <hyperlink ref="N76" r:id="rId19" xr:uid="{63C5BCC5-ABE6-B643-9455-935728CE3693}"/>
-    <hyperlink ref="N77" r:id="rId20" xr:uid="{69C7C0E5-5CEA-8D4D-9D4A-ADA6A2A65D1A}"/>
-    <hyperlink ref="N78:N82" r:id="rId21" display="https://archive.org/download/gri_c00033125012743312/gri_c00033125012743312_jp2.zip/gri_c00033125012743312_jp2%2Fgri_c00033125012743312_0063.jpg" xr:uid="{6FF12C79-E9F6-C549-9258-327FDA3A33D7}"/>
-    <hyperlink ref="N83" r:id="rId22" xr:uid="{CCCF10F0-F19D-1846-BC72-FBC8936E5C97}"/>
-    <hyperlink ref="N84:N91" r:id="rId23" display="https://archive.org/download/gri_c00033125012743312/gri_c00033125012743312_jp2.zip/gri_c00033125012743312_jp2%2Fgri_c00033125012743312_0066.jpg" xr:uid="{3597B1FC-3A1D-DB44-91DC-872A5604E1DF}"/>
-    <hyperlink ref="N92" r:id="rId24" xr:uid="{59A6F9AA-F857-E24E-9A01-92E6D0CC54B9}"/>
-    <hyperlink ref="N93:N100" r:id="rId25" display="https://archive.org/download/gri_c00033125012743312/gri_c00033125012743312_jp2.zip/gri_c00033125012743312_jp2%2Fgri_c00033125012743312_0069.jpg" xr:uid="{640913D3-144C-7041-ABD6-10B17C79F2CC}"/>
-    <hyperlink ref="N101" r:id="rId26" xr:uid="{587D31B9-4F61-064F-B3E1-BFA5BA05ABC3}"/>
+    <hyperlink ref="O10" r:id="rId1" xr:uid="{8D2C38B8-FFB6-5E49-9C32-FD70F8BF5C70}"/>
+    <hyperlink ref="O11:O17" r:id="rId2" display="https://archive.org/download/gri_c00033125012743312/gri_c00033125012743312_jp2.zip/gri_c00033125012743312_jp2%2Fgri_c00033125012743312_0033.jpg" xr:uid="{CB684880-C13B-A948-B28B-D0F22E6D61DB}"/>
+    <hyperlink ref="O18" r:id="rId3" xr:uid="{3D2A0FB2-ABE1-0849-80C3-D3CD01B0995F}"/>
+    <hyperlink ref="O19:O24" r:id="rId4" display="https://archive.org/download/gri_c00033125012743312/gri_c00033125012743312_jp2.zip/gri_c00033125012743312_jp2%2Fgri_c00033125012743312_0037.jpg" xr:uid="{0D5118B9-BCC7-3146-A3F3-B5576F2C73D3}"/>
+    <hyperlink ref="O25" r:id="rId5" xr:uid="{DEBB1F8F-01AA-1446-B6AD-CEEDB824B545}"/>
+    <hyperlink ref="O26:O35" r:id="rId6" display="https://archive.org/download/gri_c00033125012743312/gri_c00033125012743312_jp2.zip/gri_c00033125012743312_jp2%2Fgri_c00033125012743312_0041.jpg" xr:uid="{F31D613A-AAF3-5F4F-BE00-BC67B616D348}"/>
+    <hyperlink ref="O36" r:id="rId7" xr:uid="{A965DEFD-E821-B747-8F47-763DB6CFCDA5}"/>
+    <hyperlink ref="O37:O45" r:id="rId8" display="https://archive.org/download/gri_c00033125012743312/gri_c00033125012743312_jp2.zip/gri_c00033125012743312_jp2%2Fgri_c00033125012743312_0045.jpg" xr:uid="{90FBAD6C-4314-4648-999A-9318848CD478}"/>
+    <hyperlink ref="O46" r:id="rId9" xr:uid="{F38B3821-6B78-8245-AA5F-A171E6732863}"/>
+    <hyperlink ref="O47" r:id="rId10" xr:uid="{1145454B-D921-BA4D-A02B-1249ECB515EB}"/>
+    <hyperlink ref="O48:O54" r:id="rId11" display="https://archive.org/download/gri_c00033125012743312/gri_c00033125012743312_jp2.zip/gri_c00033125012743312_jp2%2Fgri_c00033125012743312_0049.jpg" xr:uid="{68184C3E-4B1F-1642-9D16-DA249976B264}"/>
+    <hyperlink ref="O55" r:id="rId12" xr:uid="{900CB1B8-822D-2B46-A8F0-8E6E907F177D}"/>
+    <hyperlink ref="O56:O62" r:id="rId13" display="https://archive.org/download/gri_c00033125012743312/gri_c00033125012743312_jp2.zip/gri_c00033125012743312_jp2%2Fgri_c00033125012743312_0052.jpg" xr:uid="{14CEA8D5-83CC-1D48-8FFA-2BE840D0DEAD}"/>
+    <hyperlink ref="O63" r:id="rId14" xr:uid="{B8EDAC7D-15E7-B44C-8207-76FC3D6F981C}"/>
+    <hyperlink ref="O64:O68" r:id="rId15" display="https://archive.org/download/gri_c00033125012743312/gri_c00033125012743312_jp2.zip/gri_c00033125012743312_jp2%2Fgri_c00033125012743312_0056.jpg" xr:uid="{747F0C47-4978-3A42-ADEC-D041490CFC3A}"/>
+    <hyperlink ref="O69" r:id="rId16" xr:uid="{53230F16-35CB-ED46-AE27-7C0C06930D06}"/>
+    <hyperlink ref="O70" r:id="rId17" xr:uid="{144055C7-22F3-0F40-844D-D61E3E061E70}"/>
+    <hyperlink ref="O71:O75" r:id="rId18" display="https://archive.org/download/gri_c00033125012743312/gri_c00033125012743312_jp2.zip/gri_c00033125012743312_jp2%2Fgri_c00033125012743312_0059.jpg" xr:uid="{A477BA26-9910-4646-AECB-B39F82D546EC}"/>
+    <hyperlink ref="O76" r:id="rId19" xr:uid="{63C5BCC5-ABE6-B643-9455-935728CE3693}"/>
+    <hyperlink ref="O77" r:id="rId20" xr:uid="{69C7C0E5-5CEA-8D4D-9D4A-ADA6A2A65D1A}"/>
+    <hyperlink ref="O78:O82" r:id="rId21" display="https://archive.org/download/gri_c00033125012743312/gri_c00033125012743312_jp2.zip/gri_c00033125012743312_jp2%2Fgri_c00033125012743312_0063.jpg" xr:uid="{6FF12C79-E9F6-C549-9258-327FDA3A33D7}"/>
+    <hyperlink ref="O83" r:id="rId22" xr:uid="{CCCF10F0-F19D-1846-BC72-FBC8936E5C97}"/>
+    <hyperlink ref="O84:O91" r:id="rId23" display="https://archive.org/download/gri_c00033125012743312/gri_c00033125012743312_jp2.zip/gri_c00033125012743312_jp2%2Fgri_c00033125012743312_0066.jpg" xr:uid="{3597B1FC-3A1D-DB44-91DC-872A5604E1DF}"/>
+    <hyperlink ref="O92" r:id="rId24" xr:uid="{59A6F9AA-F857-E24E-9A01-92E6D0CC54B9}"/>
+    <hyperlink ref="O93:O100" r:id="rId25" display="https://archive.org/download/gri_c00033125012743312/gri_c00033125012743312_jp2.zip/gri_c00033125012743312_jp2%2Fgri_c00033125012743312_0069.jpg" xr:uid="{640913D3-144C-7041-ABD6-10B17C79F2CC}"/>
+    <hyperlink ref="O101" r:id="rId26" xr:uid="{587D31B9-4F61-064F-B3E1-BFA5BA05ABC3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>